<commit_message>
analysis on sliding window
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data/mornings.xlsx
+++ b/restaurant_analytics/data/mornings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5C3060-EA46-4894-BB0A-22B8054806DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7F7D8-9217-4EF5-9404-AF5BCD6CE808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -864,9 +864,9 @@
   </sheetPr>
   <dimension ref="A1:K553"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G503" sqref="G503"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A506" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D529" sqref="D513:D529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14253,7 +14253,7 @@
         <v>33</v>
       </c>
       <c r="E507" s="11">
-        <v>82.6</v>
+        <v>84.4</v>
       </c>
       <c r="F507" s="11">
         <v>0</v>
@@ -14262,7 +14262,7 @@
         <v>0</v>
       </c>
       <c r="H507" s="11">
-        <v>12.5</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="508" spans="1:8" x14ac:dyDescent="0.25">
@@ -14279,16 +14279,16 @@
         <v>52</v>
       </c>
       <c r="E508" s="11">
-        <v>82.9</v>
+        <v>83.1</v>
       </c>
       <c r="F508" s="11">
-        <v>5.5E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="G508" s="11">
         <v>0</v>
       </c>
       <c r="H508" s="11">
-        <v>10.5</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="509" spans="1:8" x14ac:dyDescent="0.25">
@@ -14305,16 +14305,16 @@
         <v>17</v>
       </c>
       <c r="E509" s="11">
-        <v>81.099999999999994</v>
+        <v>81.7</v>
       </c>
       <c r="F509" s="11">
-        <v>7.0999999999999994E-2</v>
+        <v>0.311</v>
       </c>
       <c r="G509" s="11">
         <v>0</v>
       </c>
       <c r="H509" s="11">
-        <v>9.1</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row r="510" spans="1:8" x14ac:dyDescent="0.25">
@@ -14331,10 +14331,10 @@
         <v>11</v>
       </c>
       <c r="E510" s="11">
-        <v>76.099999999999994</v>
+        <v>77.7</v>
       </c>
       <c r="F510" s="11">
-        <v>0.40200000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="G510" s="11">
         <v>0</v>
@@ -14357,7 +14357,7 @@
         <v>25</v>
       </c>
       <c r="E511" s="11">
-        <v>76.599999999999994</v>
+        <v>76.5</v>
       </c>
       <c r="F511" s="11">
         <v>0</v>
@@ -14366,7 +14366,7 @@
         <v>0</v>
       </c>
       <c r="H511" s="11">
-        <v>6.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="512" spans="1:8" x14ac:dyDescent="0.25">
@@ -14383,7 +14383,7 @@
         <v>36</v>
       </c>
       <c r="E512" s="11">
-        <v>75.599999999999994</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="F512" s="11">
         <v>0</v>
@@ -14392,10 +14392,10 @@
         <v>0</v>
       </c>
       <c r="H512" s="11">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="513" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A513" s="7">
         <v>6</v>
       </c>
@@ -14409,7 +14409,7 @@
         <v>46</v>
       </c>
       <c r="E513" s="11">
-        <v>80.400000000000006</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="F513" s="11">
         <v>0</v>
@@ -14418,10 +14418,10 @@
         <v>0</v>
       </c>
       <c r="H513" s="11">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A514" s="7">
         <v>7</v>
       </c>
@@ -14435,19 +14435,19 @@
         <v>23</v>
       </c>
       <c r="E514" s="11">
-        <v>82.2</v>
+        <v>83.7</v>
       </c>
       <c r="F514" s="11">
-        <v>0.17299999999999999</v>
+        <v>0.59099999999999997</v>
       </c>
       <c r="G514" s="11">
         <v>0</v>
       </c>
       <c r="H514" s="11">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="515" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A515" s="7">
         <v>1</v>
       </c>
@@ -14461,19 +14461,19 @@
         <v>58</v>
       </c>
       <c r="E515" s="11">
-        <v>79.7</v>
+        <v>75</v>
       </c>
       <c r="F515" s="11">
-        <v>4.0000000000000001E-3</v>
+        <v>1.6890000000000001</v>
       </c>
       <c r="G515" s="11">
         <v>0</v>
       </c>
       <c r="H515" s="11">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="516" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A516" s="7">
         <v>2</v>
       </c>
@@ -14484,25 +14484,22 @@
         <v>45887</v>
       </c>
       <c r="D516" s="16">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E516" s="11">
-        <v>81.099999999999994</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="F516" s="11">
-        <v>0.41</v>
+        <v>1.728</v>
       </c>
       <c r="G516" s="11">
         <v>0</v>
       </c>
       <c r="H516" s="11">
-        <v>7.9</v>
-      </c>
-      <c r="J516" s="11">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="517" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A517" s="7">
         <v>3</v>
       </c>
@@ -14513,25 +14510,22 @@
         <v>45888</v>
       </c>
       <c r="D517" s="16">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E517" s="11">
-        <v>77.7</v>
+        <v>73.8</v>
       </c>
       <c r="F517" s="11">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="G517" s="11">
         <v>0</v>
       </c>
       <c r="H517" s="11">
-        <v>7.8</v>
-      </c>
-      <c r="J517" s="11">
-        <v>1.1100000000000001</v>
-      </c>
-    </row>
-    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A518" s="7">
         <v>4</v>
       </c>
@@ -14542,10 +14536,10 @@
         <v>45889</v>
       </c>
       <c r="D518" s="16">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E518" s="11">
-        <v>77.7</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="F518" s="11">
         <v>0</v>
@@ -14554,13 +14548,10 @@
         <v>0</v>
       </c>
       <c r="H518" s="11">
-        <v>7.8</v>
-      </c>
-      <c r="J518" s="11">
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="519" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A519" s="7">
         <v>5</v>
       </c>
@@ -14571,10 +14562,10 @@
         <v>45890</v>
       </c>
       <c r="D519" s="16">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E519" s="11">
-        <v>73.400000000000006</v>
+        <v>70.5</v>
       </c>
       <c r="F519" s="11">
         <v>0</v>
@@ -14583,13 +14574,10 @@
         <v>0</v>
       </c>
       <c r="H519" s="11">
-        <v>9.9</v>
-      </c>
-      <c r="J519" s="11">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="520" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A520" s="7">
         <v>6</v>
       </c>
@@ -14600,10 +14588,10 @@
         <v>45891</v>
       </c>
       <c r="D520" s="16">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E520" s="11">
-        <v>73.900000000000006</v>
+        <v>72</v>
       </c>
       <c r="F520" s="11">
         <v>0</v>
@@ -14612,13 +14600,10 @@
         <v>0</v>
       </c>
       <c r="H520" s="11">
-        <v>7.8</v>
-      </c>
-      <c r="J520" s="11">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="521" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="521" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A521" s="7">
         <v>7</v>
       </c>
@@ -14629,10 +14614,10 @@
         <v>45892</v>
       </c>
       <c r="D521" s="16">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E521" s="11">
-        <v>73.8</v>
+        <v>74.7</v>
       </c>
       <c r="F521" s="11">
         <v>0</v>
@@ -14641,13 +14626,10 @@
         <v>0</v>
       </c>
       <c r="H521" s="11">
-        <v>6.4</v>
-      </c>
-      <c r="J521" s="11">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="522" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A522" s="7">
         <v>1</v>
       </c>
@@ -14658,10 +14640,10 @@
         <v>45893</v>
       </c>
       <c r="D522" s="16">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="E522" s="11">
-        <v>73.8</v>
+        <v>66.599999999999994</v>
       </c>
       <c r="F522" s="11">
         <v>0</v>
@@ -14670,13 +14652,10 @@
         <v>0</v>
       </c>
       <c r="H522" s="11">
-        <v>7.6</v>
-      </c>
-      <c r="J522" s="11">
-        <v>4.2699999999999996</v>
-      </c>
-    </row>
-    <row r="523" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="523" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A523" s="7">
         <v>2</v>
       </c>
@@ -14687,25 +14666,22 @@
         <v>45894</v>
       </c>
       <c r="D523" s="16">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E523" s="11">
-        <v>73.2</v>
+        <v>59.7</v>
       </c>
       <c r="F523" s="11">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="G523" s="11">
         <v>0</v>
       </c>
       <c r="H523" s="11">
-        <v>7.7</v>
-      </c>
-      <c r="J523" s="11">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="524" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="524" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A524" s="7">
         <v>3</v>
       </c>
@@ -14716,25 +14692,22 @@
         <v>45895</v>
       </c>
       <c r="D524" s="16">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E524" s="11">
-        <v>72.3</v>
+        <v>63.9</v>
       </c>
       <c r="F524" s="11">
-        <v>0.21</v>
+        <v>0</v>
       </c>
       <c r="G524" s="11">
         <v>0</v>
       </c>
       <c r="H524" s="11">
-        <v>8.1</v>
-      </c>
-      <c r="J524" s="11">
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="525" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="525" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A525" s="7">
         <v>4</v>
       </c>
@@ -14745,25 +14718,22 @@
         <v>45896</v>
       </c>
       <c r="D525" s="16">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E525" s="11">
-        <v>71.5</v>
+        <v>66.2</v>
       </c>
       <c r="F525" s="11">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="G525" s="11">
         <v>0</v>
       </c>
       <c r="H525" s="11">
-        <v>5</v>
-      </c>
-      <c r="J525" s="11">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="526" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="526" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A526" s="7">
         <v>5</v>
       </c>
@@ -14774,25 +14744,22 @@
         <v>45897</v>
       </c>
       <c r="D526" s="16">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E526" s="11">
-        <v>71</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F526" s="11">
-        <v>0</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="G526" s="11">
         <v>0</v>
       </c>
       <c r="H526" s="11">
-        <v>8</v>
-      </c>
-      <c r="J526" s="11">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="527" spans="1:10" x14ac:dyDescent="0.25">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="527" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A527" s="7">
         <v>6</v>
       </c>
@@ -14803,25 +14770,22 @@
         <v>45898</v>
       </c>
       <c r="D527" s="16">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E527" s="11">
-        <v>70.5</v>
+        <v>63.9</v>
       </c>
       <c r="F527" s="11">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="G527" s="11">
         <v>0</v>
       </c>
       <c r="H527" s="11">
-        <v>6</v>
-      </c>
-      <c r="J527" s="11">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="528" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="528" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A528" s="7">
         <v>7</v>
       </c>
@@ -14832,22 +14796,19 @@
         <v>45899</v>
       </c>
       <c r="D528" s="16">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="E528" s="11">
-        <v>72</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F528" s="11">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="G528" s="11">
         <v>0</v>
       </c>
       <c r="H528" s="11">
-        <v>6</v>
-      </c>
-      <c r="J528" s="11">
-        <v>0.49</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="529" spans="1:10" x14ac:dyDescent="0.25">
@@ -14861,10 +14822,10 @@
         <v>45900</v>
       </c>
       <c r="D529" s="16">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="E529" s="11">
-        <v>72.5</v>
+        <v>65.5</v>
       </c>
       <c r="F529" s="11">
         <v>0</v>
@@ -14873,10 +14834,7 @@
         <v>0</v>
       </c>
       <c r="H529" s="11">
-        <v>1</v>
-      </c>
-      <c r="J529" s="11">
-        <v>6.92</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="530" spans="1:10" x14ac:dyDescent="0.25">
@@ -14893,7 +14851,7 @@
         <v>5</v>
       </c>
       <c r="E530" s="11">
-        <v>73</v>
+        <v>68.7</v>
       </c>
       <c r="F530" s="11">
         <v>0</v>
@@ -14902,7 +14860,7 @@
         <v>0</v>
       </c>
       <c r="H530" s="11">
-        <v>2</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I530" s="10" t="s">
         <v>19</v>
@@ -14925,7 +14883,7 @@
         <v>20</v>
       </c>
       <c r="E531" s="11">
-        <v>72</v>
+        <v>70.3</v>
       </c>
       <c r="F531" s="11">
         <v>0</v>
@@ -14934,7 +14892,7 @@
         <v>0</v>
       </c>
       <c r="H531" s="11">
-        <v>7</v>
+        <v>4.2</v>
       </c>
       <c r="J531" s="11">
         <v>1.78</v>
@@ -14954,16 +14912,16 @@
         <v>22</v>
       </c>
       <c r="E532" s="11">
-        <v>71.5</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F532" s="11">
-        <v>0.13</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="G532" s="11">
         <v>0</v>
       </c>
       <c r="H532" s="11">
-        <v>9</v>
+        <v>10.4</v>
       </c>
       <c r="J532" s="11">
         <v>1.59</v>
@@ -14983,7 +14941,7 @@
         <v>30</v>
       </c>
       <c r="E533" s="11">
-        <v>72</v>
+        <v>60.6</v>
       </c>
       <c r="F533" s="11">
         <v>0</v>
@@ -14992,7 +14950,7 @@
         <v>0</v>
       </c>
       <c r="H533" s="11">
-        <v>5</v>
+        <v>9.9</v>
       </c>
       <c r="J533" s="11">
         <v>1.03</v>
@@ -15012,16 +14970,16 @@
         <v>21</v>
       </c>
       <c r="E534" s="11">
-        <v>70.5</v>
+        <v>61</v>
       </c>
       <c r="F534" s="11">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="G534" s="11">
         <v>0</v>
       </c>
       <c r="H534" s="11">
-        <v>5</v>
+        <v>12.2</v>
       </c>
       <c r="J534" s="11">
         <v>0.95</v>
@@ -15041,7 +14999,7 @@
         <v>17</v>
       </c>
       <c r="E535" s="11">
-        <v>71</v>
+        <v>59.7</v>
       </c>
       <c r="F535" s="11">
         <v>0</v>
@@ -15050,7 +15008,7 @@
         <v>0</v>
       </c>
       <c r="H535" s="11">
-        <v>4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="J535" s="11">
         <v>1.1399999999999999</v>
@@ -15070,7 +15028,7 @@
         <v>33</v>
       </c>
       <c r="E536" s="11">
-        <v>71</v>
+        <v>60.6</v>
       </c>
       <c r="F536" s="11">
         <v>0.32</v>
@@ -15079,7 +15037,7 @@
         <v>0</v>
       </c>
       <c r="H536" s="11">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="J536" s="11">
         <v>3.13</v>
@@ -15099,7 +15057,7 @@
         <v>29</v>
       </c>
       <c r="E537" s="11">
-        <v>69.5</v>
+        <v>62.6</v>
       </c>
       <c r="F537" s="11">
         <v>0.06</v>
@@ -15108,7 +15066,7 @@
         <v>0</v>
       </c>
       <c r="H537" s="11">
-        <v>8</v>
+        <v>6.4</v>
       </c>
       <c r="J537" s="11">
         <v>1.37</v>
@@ -15128,7 +15086,7 @@
         <v>15</v>
       </c>
       <c r="E538" s="11">
-        <v>68</v>
+        <v>65.3</v>
       </c>
       <c r="F538" s="11">
         <v>0</v>
@@ -15137,7 +15095,7 @@
         <v>0</v>
       </c>
       <c r="H538" s="11">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="J538" s="11">
         <v>0.64</v>
@@ -15157,7 +15115,7 @@
         <v>20</v>
       </c>
       <c r="E539" s="11">
-        <v>70.5</v>
+        <v>66.900000000000006</v>
       </c>
       <c r="F539" s="11">
         <v>0</v>
@@ -15166,7 +15124,7 @@
         <v>0</v>
       </c>
       <c r="H539" s="11">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J539" s="11">
         <v>1.34</v>
@@ -15459,8 +15417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6638D5E3-C858-457D-8856-EE1DEA6B94D7}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="R43" sqref="R43"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:XFD64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15596,7 +15554,7 @@
         <v>8.7200000000000006</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q49" si="2">O3-A3</f>
+        <f t="shared" ref="Q3:Q63" si="2">O3-A3</f>
         <v>-11</v>
       </c>
     </row>
@@ -17917,21 +17875,21 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="47" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="40">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="41">
+      <c r="B47" s="26">
         <v>45884</v>
       </c>
-      <c r="C47" s="40">
+      <c r="C47">
         <v>22</v>
       </c>
-      <c r="O47" s="42">
+      <c r="O47" s="25">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="P47" s="42">
+      <c r="P47" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -17986,23 +17944,33 @@
         <v>-42</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="29">
+    <row r="50" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="40">
+        <v>20</v>
+      </c>
+      <c r="B50" s="41">
         <v>45887</v>
       </c>
-      <c r="C50" s="28">
+      <c r="C50" s="40">
         <v>17</v>
       </c>
-      <c r="O50" s="30">
+      <c r="O50" s="42">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="P50" s="30">
+      <c r="P50" s="42">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q50" s="40">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11</v>
+      </c>
       <c r="B51" s="26">
         <v>45888</v>
       </c>
@@ -18017,8 +17985,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q51">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>8</v>
+      </c>
       <c r="B52" s="26">
         <v>45889</v>
       </c>
@@ -18033,8 +18008,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q52">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
       <c r="B53" s="26">
         <v>45890</v>
       </c>
@@ -18049,8 +18031,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q53">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>41</v>
+      </c>
       <c r="B54" s="26">
         <v>45891</v>
       </c>
@@ -18065,8 +18054,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q54">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>42</v>
+      </c>
       <c r="B55" s="26">
         <v>45892</v>
       </c>
@@ -18081,8 +18077,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q55">
+        <f t="shared" si="2"/>
+        <v>-24</v>
+      </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>78</v>
+      </c>
       <c r="B56" s="26">
         <v>45893</v>
       </c>
@@ -18097,8 +18100,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q56">
+        <f t="shared" si="2"/>
+        <v>-35</v>
+      </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11</v>
+      </c>
       <c r="B57" s="26">
         <v>45894</v>
       </c>
@@ -18113,8 +18123,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q57">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>19</v>
+      </c>
       <c r="B58" s="26">
         <v>45895</v>
       </c>
@@ -18129,8 +18146,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q58">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>27</v>
+      </c>
       <c r="B59" s="26">
         <v>45896</v>
       </c>
@@ -18145,8 +18169,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>43</v>
+      </c>
       <c r="B60" s="26">
         <v>45897</v>
       </c>
@@ -18161,8 +18192,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q60">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>51</v>
+      </c>
       <c r="B61" s="26">
         <v>45898</v>
       </c>
@@ -18177,8 +18215,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q61">
+        <f t="shared" si="2"/>
+        <v>-28</v>
+      </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>45</v>
+      </c>
       <c r="B62" s="26">
         <v>45899</v>
       </c>
@@ -18193,8 +18238,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
+      <c r="Q62">
+        <f t="shared" si="2"/>
+        <v>-28</v>
+      </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
       <c r="B63" s="26">
         <v>45900</v>
       </c>
@@ -18209,19 +18261,23 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B64" s="26">
+      <c r="Q63">
+        <f t="shared" si="2"/>
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="29">
         <v>45901</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="28">
         <v>3</v>
       </c>
-      <c r="O64" s="25">
+      <c r="O64" s="30">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="P64" s="25">
+      <c r="P64" s="30">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -18575,7 +18631,7 @@
   <conditionalFormatting sqref="C83:L83 N83">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q49">
+  <conditionalFormatting sqref="Q1:Q63">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
updating for morning data
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data/mornings.xlsx
+++ b/restaurant_analytics/data/mornings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE7F7D8-9217-4EF5-9404-AF5BCD6CE808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C989C73-F127-425F-B7C1-E3427A856D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="day">Sheet1!$A$1</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>day</t>
   </si>
@@ -435,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -524,16 +525,39 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -864,9 +888,9 @@
   </sheetPr>
   <dimension ref="A1:K553"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A506" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D529" sqref="D513:D529"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A515" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L535" sqref="L535"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14848,7 +14872,7 @@
         <v>45901</v>
       </c>
       <c r="D530" s="16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E530" s="11">
         <v>68.7</v>
@@ -14864,9 +14888,6 @@
       </c>
       <c r="I530" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="J530" s="11">
-        <v>1.48</v>
       </c>
     </row>
     <row r="531" spans="1:10" x14ac:dyDescent="0.25">
@@ -14880,7 +14901,7 @@
         <v>45902</v>
       </c>
       <c r="D531" s="16">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E531" s="11">
         <v>70.3</v>
@@ -14894,8 +14915,8 @@
       <c r="H531" s="11">
         <v>4.2</v>
       </c>
-      <c r="J531" s="11">
-        <v>1.78</v>
+      <c r="J531" s="40">
+        <v>5.4949999999999992</v>
       </c>
     </row>
     <row r="532" spans="1:10" x14ac:dyDescent="0.25">
@@ -14909,7 +14930,7 @@
         <v>45903</v>
       </c>
       <c r="D532" s="16">
-        <v>22</v>
+        <v>18.5</v>
       </c>
       <c r="E532" s="11">
         <v>66.900000000000006</v>
@@ -14923,8 +14944,8 @@
       <c r="H532" s="11">
         <v>10.4</v>
       </c>
-      <c r="J532" s="11">
-        <v>1.59</v>
+      <c r="J532" s="40">
+        <v>3.0949999999999998</v>
       </c>
     </row>
     <row r="533" spans="1:10" x14ac:dyDescent="0.25">
@@ -14938,7 +14959,7 @@
         <v>45904</v>
       </c>
       <c r="D533" s="16">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E533" s="11">
         <v>60.6</v>
@@ -14952,8 +14973,8 @@
       <c r="H533" s="11">
         <v>9.9</v>
       </c>
-      <c r="J533" s="11">
-        <v>1.03</v>
+      <c r="J533" s="40">
+        <v>5.6</v>
       </c>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.25">
@@ -14967,7 +14988,7 @@
         <v>45905</v>
       </c>
       <c r="D534" s="16">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="E534" s="11">
         <v>61</v>
@@ -14981,8 +15002,8 @@
       <c r="H534" s="11">
         <v>12.2</v>
       </c>
-      <c r="J534" s="11">
-        <v>0.95</v>
+      <c r="J534" s="40">
+        <v>3.9899999999999998</v>
       </c>
     </row>
     <row r="535" spans="1:10" x14ac:dyDescent="0.25">
@@ -14996,7 +15017,7 @@
         <v>45906</v>
       </c>
       <c r="D535" s="16">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E535" s="11">
         <v>59.7</v>
@@ -15010,8 +15031,8 @@
       <c r="H535" s="11">
         <v>9.3000000000000007</v>
       </c>
-      <c r="J535" s="11">
-        <v>1.1399999999999999</v>
+      <c r="J535" s="40">
+        <v>4.7050000000000001</v>
       </c>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.25">
@@ -15025,7 +15046,7 @@
         <v>45907</v>
       </c>
       <c r="D536" s="16">
-        <v>33</v>
+        <v>36.5</v>
       </c>
       <c r="E536" s="11">
         <v>60.6</v>
@@ -15039,8 +15060,8 @@
       <c r="H536" s="11">
         <v>7.3</v>
       </c>
-      <c r="J536" s="11">
-        <v>3.13</v>
+      <c r="J536" s="40">
+        <v>3.4649999999999999</v>
       </c>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.25">
@@ -15054,7 +15075,7 @@
         <v>45908</v>
       </c>
       <c r="D537" s="16">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E537" s="11">
         <v>62.6</v>
@@ -15068,8 +15089,8 @@
       <c r="H537" s="11">
         <v>6.4</v>
       </c>
-      <c r="J537" s="11">
-        <v>1.37</v>
+      <c r="J537" s="40">
+        <v>2.98</v>
       </c>
     </row>
     <row r="538" spans="1:10" x14ac:dyDescent="0.25">
@@ -15083,7 +15104,7 @@
         <v>45909</v>
       </c>
       <c r="D538" s="16">
-        <v>15</v>
+        <v>23.5</v>
       </c>
       <c r="E538" s="11">
         <v>65.3</v>
@@ -15097,8 +15118,8 @@
       <c r="H538" s="11">
         <v>7.5</v>
       </c>
-      <c r="J538" s="11">
-        <v>0.64</v>
+      <c r="J538" s="40">
+        <v>2.1749999999999998</v>
       </c>
     </row>
     <row r="539" spans="1:10" x14ac:dyDescent="0.25">
@@ -15112,7 +15133,7 @@
         <v>45910</v>
       </c>
       <c r="D539" s="16">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E539" s="11">
         <v>66.900000000000006</v>
@@ -15126,8 +15147,8 @@
       <c r="H539" s="11">
         <v>8</v>
       </c>
-      <c r="J539" s="11">
-        <v>1.34</v>
+      <c r="J539" s="40">
+        <v>3.2949999999999999</v>
       </c>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.25">
@@ -15141,7 +15162,7 @@
         <v>45911</v>
       </c>
       <c r="D540" s="16">
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="E540" s="11">
         <v>69</v>
@@ -15155,8 +15176,8 @@
       <c r="H540" s="11">
         <v>6</v>
       </c>
-      <c r="J540" s="11">
-        <v>1.1100000000000001</v>
+      <c r="J540" s="40">
+        <v>2.33</v>
       </c>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.25">
@@ -15170,7 +15191,7 @@
         <v>45912</v>
       </c>
       <c r="D541" s="16">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E541" s="11">
         <v>70</v>
@@ -15184,8 +15205,8 @@
       <c r="H541" s="11">
         <v>4</v>
       </c>
-      <c r="J541" s="11">
-        <v>2.8</v>
+      <c r="J541" s="40">
+        <v>4.0549999999999997</v>
       </c>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.25">
@@ -15199,7 +15220,7 @@
         <v>45913</v>
       </c>
       <c r="D542" s="16">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E542" s="11">
         <v>69</v>
@@ -15213,8 +15234,8 @@
       <c r="H542" s="11">
         <v>8</v>
       </c>
-      <c r="J542" s="11">
-        <v>2.5499999999999998</v>
+      <c r="J542" s="40">
+        <v>4.9399999999999995</v>
       </c>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.25">
@@ -15228,7 +15249,7 @@
         <v>45914</v>
       </c>
       <c r="D543" s="16">
-        <v>49</v>
+        <v>48.5</v>
       </c>
       <c r="E543" s="11">
         <v>70</v>
@@ -15242,8 +15263,8 @@
       <c r="H543" s="11">
         <v>4</v>
       </c>
-      <c r="J543" s="11">
-        <v>7.65</v>
+      <c r="J543" s="40">
+        <v>15.91</v>
       </c>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.25">
@@ -15257,7 +15278,7 @@
         <v>45915</v>
       </c>
       <c r="D544" s="16">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E544" s="11">
         <v>56.5</v>
@@ -15271,8 +15292,8 @@
       <c r="H544" s="11">
         <v>10</v>
       </c>
-      <c r="J544" s="11">
-        <v>1.79</v>
+      <c r="J544" s="40">
+        <v>3.6150000000000002</v>
       </c>
     </row>
     <row r="545" spans="1:10" x14ac:dyDescent="0.25">
@@ -15286,7 +15307,7 @@
         <v>45916</v>
       </c>
       <c r="D545" s="16">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E545" s="11">
         <v>57</v>
@@ -15300,8 +15321,8 @@
       <c r="H545" s="11">
         <v>2</v>
       </c>
-      <c r="J545" s="11">
-        <v>3.53</v>
+      <c r="J545" s="40">
+        <v>4.03</v>
       </c>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.25">
@@ -15315,7 +15336,7 @@
         <v>45917</v>
       </c>
       <c r="D546" s="16">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E546" s="11">
         <v>58.5</v>
@@ -15329,8 +15350,8 @@
       <c r="H546" s="11">
         <v>5</v>
       </c>
-      <c r="J546" s="11">
-        <v>2.98</v>
+      <c r="J546" s="40">
+        <v>4.57</v>
       </c>
     </row>
     <row r="547" spans="1:10" x14ac:dyDescent="0.25">
@@ -15344,7 +15365,7 @@
         <v>45918</v>
       </c>
       <c r="D547" s="16">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E547" s="11">
         <v>59.5</v>
@@ -15358,8 +15379,8 @@
       <c r="H547" s="11">
         <v>8</v>
       </c>
-      <c r="J547" s="11">
-        <v>1.64</v>
+      <c r="J547" s="40">
+        <v>2.9950000000000001</v>
       </c>
     </row>
     <row r="548" spans="1:10" x14ac:dyDescent="0.25">
@@ -15373,7 +15394,7 @@
         <v>45919</v>
       </c>
       <c r="D548" s="16">
-        <v>18</v>
+        <v>31.5</v>
       </c>
       <c r="E548" s="11">
         <v>61</v>
@@ -15387,8 +15408,8 @@
       <c r="H548" s="11">
         <v>9</v>
       </c>
-      <c r="J548" s="11">
-        <v>2.2999999999999998</v>
+      <c r="J548" s="40">
+        <v>5.34</v>
       </c>
     </row>
     <row r="549" spans="1:10" x14ac:dyDescent="0.25">
@@ -15417,8 +15438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6638D5E3-C858-457D-8856-EE1DEA6B94D7}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="P65" sqref="P65:P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17944,25 +17965,25 @@
         <v>-42</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="40">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>20</v>
       </c>
-      <c r="B50" s="41">
+      <c r="B50" s="26">
         <v>45887</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50">
         <v>17</v>
       </c>
-      <c r="O50" s="42">
+      <c r="O50" s="25">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="P50" s="42">
+      <c r="P50" s="25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="Q50" s="40">
+      <c r="Q50">
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
@@ -18271,15 +18292,30 @@
         <v>45901</v>
       </c>
       <c r="C64" s="28">
-        <v>3</v>
+        <v>21</v>
+      </c>
+      <c r="D64" s="28">
+        <v>34</v>
+      </c>
+      <c r="E64" s="28">
+        <v>18</v>
+      </c>
+      <c r="F64" s="28">
+        <v>16</v>
+      </c>
+      <c r="G64" s="28">
+        <v>17</v>
+      </c>
+      <c r="H64" s="28">
+        <v>17</v>
       </c>
       <c r="O64" s="30">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="P64" s="30">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.25">
@@ -18287,15 +18323,30 @@
         <v>45902</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="D65">
+        <v>33</v>
+      </c>
+      <c r="E65">
+        <v>21</v>
+      </c>
+      <c r="F65">
+        <v>16</v>
+      </c>
+      <c r="G65">
+        <v>25</v>
+      </c>
+      <c r="H65">
+        <v>24</v>
       </c>
       <c r="O65" s="25">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="P65" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.25">
@@ -18303,15 +18354,30 @@
         <v>45903</v>
       </c>
       <c r="C66">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="D66">
+        <v>18</v>
+      </c>
+      <c r="E66">
+        <v>18</v>
+      </c>
+      <c r="F66">
+        <v>12</v>
+      </c>
+      <c r="G66">
+        <v>14</v>
+      </c>
+      <c r="H66">
+        <v>20</v>
       </c>
       <c r="O66" s="25">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="P66" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.69</v>
       </c>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.25">
@@ -18319,15 +18385,30 @@
         <v>45904</v>
       </c>
       <c r="C67">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="D67">
+        <v>26</v>
+      </c>
+      <c r="E67">
+        <v>22</v>
+      </c>
+      <c r="F67">
+        <v>30</v>
+      </c>
+      <c r="G67">
+        <v>19</v>
+      </c>
+      <c r="H67">
+        <v>27</v>
       </c>
       <c r="O67" s="25">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="P67" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.25">
@@ -18335,15 +18416,30 @@
         <v>45905</v>
       </c>
       <c r="C68">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D68">
+        <v>39</v>
+      </c>
+      <c r="E68">
+        <v>35</v>
+      </c>
+      <c r="F68">
+        <v>35</v>
+      </c>
+      <c r="G68">
+        <v>34</v>
+      </c>
+      <c r="H68">
+        <v>36</v>
       </c>
       <c r="O68" s="25">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="P68" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.25">
@@ -18351,15 +18447,30 @@
         <v>45906</v>
       </c>
       <c r="C69">
-        <v>16</v>
+        <v>40</v>
+      </c>
+      <c r="D69">
+        <v>49</v>
+      </c>
+      <c r="E69">
+        <v>48</v>
+      </c>
+      <c r="F69">
+        <v>34</v>
+      </c>
+      <c r="G69">
+        <v>32</v>
+      </c>
+      <c r="H69">
+        <v>33</v>
       </c>
       <c r="O69" s="25">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="P69" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>6.96</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.25">
@@ -18367,15 +18478,30 @@
         <v>45907</v>
       </c>
       <c r="C70">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <v>33</v>
+      </c>
+      <c r="E70">
+        <v>36</v>
+      </c>
+      <c r="F70">
+        <v>36</v>
+      </c>
+      <c r="G70">
         <v>29</v>
+      </c>
+      <c r="H70">
+        <v>34</v>
       </c>
       <c r="O70" s="25">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P70" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.25">
@@ -18383,15 +18509,30 @@
         <v>45908</v>
       </c>
       <c r="C71">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="D71">
+        <v>29</v>
+      </c>
+      <c r="E71">
+        <v>23</v>
+      </c>
+      <c r="F71">
+        <v>20</v>
+      </c>
+      <c r="G71">
+        <v>17</v>
+      </c>
+      <c r="H71">
+        <v>20</v>
       </c>
       <c r="O71" s="25">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="P71" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3.73</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.25">
@@ -18399,15 +18540,30 @@
         <v>45909</v>
       </c>
       <c r="C72">
-        <v>14</v>
+        <v>24</v>
+      </c>
+      <c r="D72">
+        <v>25</v>
+      </c>
+      <c r="E72">
+        <v>23</v>
+      </c>
+      <c r="F72">
+        <v>18</v>
+      </c>
+      <c r="G72">
+        <v>20</v>
+      </c>
+      <c r="H72">
+        <v>20</v>
       </c>
       <c r="O72" s="25">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="P72" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.25">
@@ -18415,15 +18571,30 @@
         <v>45910</v>
       </c>
       <c r="C73">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="D73">
+        <v>20</v>
+      </c>
+      <c r="E73">
+        <v>24</v>
+      </c>
+      <c r="F73">
+        <v>26</v>
+      </c>
+      <c r="G73">
+        <v>19</v>
+      </c>
+      <c r="H73">
+        <v>20</v>
       </c>
       <c r="O73" s="25">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="P73" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.52</v>
       </c>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.25">
@@ -18431,15 +18602,30 @@
         <v>45911</v>
       </c>
       <c r="C74">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="D74">
+        <v>23</v>
+      </c>
+      <c r="E74">
+        <v>28</v>
+      </c>
+      <c r="F74">
+        <v>23</v>
+      </c>
+      <c r="G74">
+        <v>24</v>
+      </c>
+      <c r="H74">
+        <v>26</v>
       </c>
       <c r="O74" s="25">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="P74" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.25">
@@ -18447,15 +18633,30 @@
         <v>45912</v>
       </c>
       <c r="C75">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="D75">
+        <v>26</v>
+      </c>
+      <c r="E75">
+        <v>20</v>
+      </c>
+      <c r="F75">
+        <v>22</v>
+      </c>
+      <c r="G75">
+        <v>26</v>
+      </c>
+      <c r="H75">
+        <v>22</v>
       </c>
       <c r="O75" s="25">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="P75" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.25">
@@ -18463,15 +18664,30 @@
         <v>45913</v>
       </c>
       <c r="C76">
+        <v>37</v>
+      </c>
+      <c r="D76">
+        <v>32</v>
+      </c>
+      <c r="E76">
+        <v>43</v>
+      </c>
+      <c r="F76">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <v>31</v>
+      </c>
+      <c r="H76">
         <v>24</v>
       </c>
       <c r="O76" s="25">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="P76" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.25">
@@ -18479,15 +18695,30 @@
         <v>45914</v>
       </c>
       <c r="C77">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="D77">
+        <v>43</v>
+      </c>
+      <c r="E77">
+        <v>24</v>
+      </c>
+      <c r="F77">
+        <v>32</v>
+      </c>
+      <c r="G77">
+        <v>51</v>
+      </c>
+      <c r="H77">
+        <v>62</v>
       </c>
       <c r="O77" s="25">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="P77" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>12.32</v>
       </c>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.25">
@@ -18495,15 +18726,30 @@
         <v>45915</v>
       </c>
       <c r="C78">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="D78">
+        <v>26</v>
+      </c>
+      <c r="E78">
+        <v>25</v>
+      </c>
+      <c r="F78">
+        <v>16</v>
+      </c>
+      <c r="G78">
+        <v>14</v>
+      </c>
+      <c r="H78">
+        <v>13</v>
       </c>
       <c r="O78" s="25">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="P78" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.25">
@@ -18511,15 +18757,30 @@
         <v>45916</v>
       </c>
       <c r="C79">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="D79">
+        <v>40</v>
+      </c>
+      <c r="E79">
+        <v>29</v>
+      </c>
+      <c r="F79">
+        <v>25</v>
+      </c>
+      <c r="G79">
+        <v>25</v>
+      </c>
+      <c r="H79">
+        <v>21</v>
       </c>
       <c r="O79" s="25">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="P79" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>5.96</v>
       </c>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.25">
@@ -18527,15 +18788,30 @@
         <v>45917</v>
       </c>
       <c r="C80">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="D80">
+        <v>23</v>
+      </c>
+      <c r="E80">
+        <v>25</v>
+      </c>
+      <c r="F80">
+        <v>27</v>
+      </c>
+      <c r="G80">
+        <v>15</v>
+      </c>
+      <c r="H80">
+        <v>18</v>
       </c>
       <c r="O80" s="25">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="P80" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:16" x14ac:dyDescent="0.25">
@@ -18543,15 +18819,30 @@
         <v>45918</v>
       </c>
       <c r="C81">
+        <v>27</v>
+      </c>
+      <c r="D81">
+        <v>18</v>
+      </c>
+      <c r="E81">
+        <v>27</v>
+      </c>
+      <c r="F81">
         <v>20</v>
+      </c>
+      <c r="G81">
+        <v>20</v>
+      </c>
+      <c r="H81">
+        <v>24</v>
       </c>
       <c r="O81" s="25">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="P81" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="2:16" x14ac:dyDescent="0.25">
@@ -18559,15 +18850,30 @@
         <v>45919</v>
       </c>
       <c r="C82">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c r="D82">
+        <v>34</v>
+      </c>
+      <c r="E82">
+        <v>30</v>
+      </c>
+      <c r="F82">
+        <v>32</v>
+      </c>
+      <c r="G82">
+        <v>20</v>
+      </c>
+      <c r="H82">
+        <v>24</v>
       </c>
       <c r="O82" s="25">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="P82" s="25">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4.78</v>
       </c>
     </row>
     <row r="83" spans="2:16" x14ac:dyDescent="0.25">
@@ -18575,7 +18881,3489 @@
         <v>41</v>
       </c>
       <c r="C83" s="34">
-        <v>24.96</v>
+        <v>22.74</v>
+      </c>
+      <c r="D83" s="34">
+        <v>20.34</v>
+      </c>
+      <c r="E83" s="34">
+        <v>20.07</v>
+      </c>
+      <c r="F83" s="34">
+        <v>21.27</v>
+      </c>
+      <c r="G83" s="34">
+        <v>29.86</v>
+      </c>
+      <c r="H83" s="33">
+        <v>24.14</v>
+      </c>
+      <c r="I83" s="34"/>
+      <c r="J83" s="34"/>
+      <c r="K83" s="34"/>
+      <c r="L83" s="34"/>
+      <c r="M83" s="34"/>
+      <c r="N83" s="35"/>
+      <c r="O83" s="36">
+        <f>ROUND(AVERAGE(C83:N83),2)</f>
+        <v>23.07</v>
+      </c>
+      <c r="P83" s="36">
+        <f>ROUND(_xlfn.STDEV.P(D83:O83),2)</f>
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B84" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C84" s="18">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="D84" s="18">
+        <v>18.82</v>
+      </c>
+      <c r="E84" s="18">
+        <v>20.23</v>
+      </c>
+      <c r="F84" s="18">
+        <v>17.29</v>
+      </c>
+      <c r="G84" s="18">
+        <v>16.02</v>
+      </c>
+      <c r="H84" s="22"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="19"/>
+      <c r="O84" s="25">
+        <f>ROUND(AVERAGE(C84:N84),2)</f>
+        <v>17.940000000000001</v>
+      </c>
+      <c r="P84" s="25">
+        <f>ROUND(_xlfn.STDEV.P(D84:O84),2)</f>
+        <v>1.42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:N1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C83:L83 N83">
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1:Q63">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2573A6AB-8DBE-4210-8EFE-4E449AA3F45B}">
+  <dimension ref="A1:Q84"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P65" sqref="P65:P82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="37">
+        <v>0.85</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2" s="26">
+        <v>45839</v>
+      </c>
+      <c r="C2" s="18">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>23</v>
+      </c>
+      <c r="F2">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>14</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>19</v>
+      </c>
+      <c r="N2">
+        <v>21</v>
+      </c>
+      <c r="O2" s="25">
+        <f t="shared" ref="O2:O65" si="0">ROUND(AVERAGE(C2:N2),0)</f>
+        <v>18</v>
+      </c>
+      <c r="P2" s="25">
+        <f t="shared" ref="P2:P65" si="1">ROUND(_xlfn.STDEV.P(D2:O2),2)</f>
+        <v>4.51</v>
+      </c>
+      <c r="Q2">
+        <f>O2-A2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>25</v>
+      </c>
+      <c r="B3" s="26">
+        <v>45840</v>
+      </c>
+      <c r="C3" s="18">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>24</v>
+      </c>
+      <c r="O3" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P3" s="25">
+        <f t="shared" si="1"/>
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q63" si="2">O3-A3</f>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="26">
+        <v>45841</v>
+      </c>
+      <c r="C4" s="18">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>29</v>
+      </c>
+      <c r="I4">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>31</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
+      </c>
+      <c r="N4">
+        <v>19</v>
+      </c>
+      <c r="O4" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P4" s="25">
+        <f t="shared" si="1"/>
+        <v>7.02</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="26">
+        <v>45842</v>
+      </c>
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P5" s="25">
+        <f t="shared" si="1"/>
+        <v>5.66</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" s="26">
+        <v>45843</v>
+      </c>
+      <c r="C6" s="18">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>-7</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P6" s="25">
+        <f t="shared" si="1"/>
+        <v>5.9</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" s="26">
+        <v>45844</v>
+      </c>
+      <c r="C7" s="18">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>17</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>8</v>
+      </c>
+      <c r="O7" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P7" s="25">
+        <f t="shared" si="1"/>
+        <v>5.36</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="2"/>
+        <v>-41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>13</v>
+      </c>
+      <c r="B8" s="26">
+        <v>45845</v>
+      </c>
+      <c r="C8" s="18">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>21</v>
+      </c>
+      <c r="H8">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>34</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>39</v>
+      </c>
+      <c r="N8">
+        <v>23</v>
+      </c>
+      <c r="O8" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P8" s="25">
+        <f t="shared" si="1"/>
+        <v>9.17</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>12</v>
+      </c>
+      <c r="B9" s="26">
+        <v>45846</v>
+      </c>
+      <c r="C9" s="18">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>79</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>16</v>
+      </c>
+      <c r="J9">
+        <v>29</v>
+      </c>
+      <c r="K9">
+        <v>23</v>
+      </c>
+      <c r="L9">
+        <v>48</v>
+      </c>
+      <c r="M9">
+        <v>78</v>
+      </c>
+      <c r="N9">
+        <v>36</v>
+      </c>
+      <c r="O9" s="25">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="P9" s="25">
+        <f t="shared" si="1"/>
+        <v>19.93</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>10</v>
+      </c>
+      <c r="B10" s="26">
+        <v>45847</v>
+      </c>
+      <c r="C10" s="18">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>34</v>
+      </c>
+      <c r="E10">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>27</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>29</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>28</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>31</v>
+      </c>
+      <c r="M10">
+        <v>26</v>
+      </c>
+      <c r="N10">
+        <v>21</v>
+      </c>
+      <c r="O10" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P10" s="25">
+        <f t="shared" si="1"/>
+        <v>4.83</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>25</v>
+      </c>
+      <c r="B11" s="26">
+        <v>45848</v>
+      </c>
+      <c r="C11" s="18">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>41</v>
+      </c>
+      <c r="E11">
+        <v>37</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>29</v>
+      </c>
+      <c r="I11">
+        <v>20</v>
+      </c>
+      <c r="J11">
+        <v>43</v>
+      </c>
+      <c r="K11">
+        <v>26</v>
+      </c>
+      <c r="L11">
+        <v>28</v>
+      </c>
+      <c r="M11">
+        <v>31</v>
+      </c>
+      <c r="N11">
+        <v>25</v>
+      </c>
+      <c r="O11" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="P11" s="25">
+        <f t="shared" si="1"/>
+        <v>7.15</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>29</v>
+      </c>
+      <c r="B12" s="26">
+        <v>45849</v>
+      </c>
+      <c r="C12" s="18">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>10</v>
+      </c>
+      <c r="J12">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <v>17</v>
+      </c>
+      <c r="M12">
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <v>14</v>
+      </c>
+      <c r="O12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P12" s="25">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>43</v>
+      </c>
+      <c r="B13" s="26">
+        <v>45850</v>
+      </c>
+      <c r="C13" s="18">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <v>21</v>
+      </c>
+      <c r="E13">
+        <v>36</v>
+      </c>
+      <c r="F13">
+        <v>19</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>29</v>
+      </c>
+      <c r="J13">
+        <v>45</v>
+      </c>
+      <c r="K13">
+        <v>36</v>
+      </c>
+      <c r="L13">
+        <v>19</v>
+      </c>
+      <c r="M13">
+        <v>23</v>
+      </c>
+      <c r="N13">
+        <v>30</v>
+      </c>
+      <c r="O13" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P13" s="25">
+        <f t="shared" si="1"/>
+        <v>9.2899999999999991</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>32</v>
+      </c>
+      <c r="B14" s="26">
+        <v>45851</v>
+      </c>
+      <c r="C14" s="18">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>17</v>
+      </c>
+      <c r="G14">
+        <v>17</v>
+      </c>
+      <c r="H14">
+        <v>21</v>
+      </c>
+      <c r="I14">
+        <v>22</v>
+      </c>
+      <c r="J14">
+        <v>21</v>
+      </c>
+      <c r="K14">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>42</v>
+      </c>
+      <c r="M14">
+        <v>28</v>
+      </c>
+      <c r="N14">
+        <v>28</v>
+      </c>
+      <c r="O14" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P14" s="25">
+        <f t="shared" si="1"/>
+        <v>6.71</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>20</v>
+      </c>
+      <c r="B15" s="26">
+        <v>45852</v>
+      </c>
+      <c r="C15" s="18">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>23</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <v>19</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>23</v>
+      </c>
+      <c r="J15">
+        <v>18</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <v>32</v>
+      </c>
+      <c r="N15">
+        <v>33</v>
+      </c>
+      <c r="O15" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P15" s="25">
+        <f t="shared" si="1"/>
+        <v>5.64</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>11</v>
+      </c>
+      <c r="B16" s="26">
+        <v>45853</v>
+      </c>
+      <c r="C16" s="18">
+        <v>44</v>
+      </c>
+      <c r="D16">
+        <v>42</v>
+      </c>
+      <c r="E16">
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <v>35</v>
+      </c>
+      <c r="G16">
+        <v>39</v>
+      </c>
+      <c r="H16">
+        <v>79</v>
+      </c>
+      <c r="I16">
+        <v>38</v>
+      </c>
+      <c r="J16">
+        <v>75</v>
+      </c>
+      <c r="K16">
+        <v>36</v>
+      </c>
+      <c r="L16">
+        <v>44</v>
+      </c>
+      <c r="M16">
+        <v>37</v>
+      </c>
+      <c r="N16">
+        <v>36</v>
+      </c>
+      <c r="O16" s="25">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P16" s="25">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
+        <v>27</v>
+      </c>
+      <c r="B17" s="26">
+        <v>45854</v>
+      </c>
+      <c r="C17" s="18">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>22</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>18</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <v>30</v>
+      </c>
+      <c r="K17">
+        <v>22</v>
+      </c>
+      <c r="L17">
+        <v>22</v>
+      </c>
+      <c r="M17">
+        <v>21</v>
+      </c>
+      <c r="N17">
+        <v>12</v>
+      </c>
+      <c r="O17" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P17" s="25">
+        <f t="shared" si="1"/>
+        <v>5.51</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>15</v>
+      </c>
+      <c r="B18" s="26">
+        <v>45855</v>
+      </c>
+      <c r="C18" s="18">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>26</v>
+      </c>
+      <c r="F18">
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>19</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>24</v>
+      </c>
+      <c r="L18">
+        <v>25</v>
+      </c>
+      <c r="M18">
+        <v>47</v>
+      </c>
+      <c r="N18">
+        <v>18</v>
+      </c>
+      <c r="O18" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P18" s="25">
+        <f t="shared" si="1"/>
+        <v>8.02</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
+        <v>27</v>
+      </c>
+      <c r="B19" s="26">
+        <v>45856</v>
+      </c>
+      <c r="C19" s="18">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>16</v>
+      </c>
+      <c r="F19">
+        <v>17</v>
+      </c>
+      <c r="G19">
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <v>17</v>
+      </c>
+      <c r="K19">
+        <v>16</v>
+      </c>
+      <c r="L19">
+        <v>20</v>
+      </c>
+      <c r="M19">
+        <v>19</v>
+      </c>
+      <c r="N19">
+        <v>6</v>
+      </c>
+      <c r="O19" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P19" s="25">
+        <f t="shared" si="1"/>
+        <v>4.01</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>35</v>
+      </c>
+      <c r="B20" s="26">
+        <v>45857</v>
+      </c>
+      <c r="C20" s="18">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>34</v>
+      </c>
+      <c r="F20">
+        <v>24</v>
+      </c>
+      <c r="G20">
+        <v>17</v>
+      </c>
+      <c r="H20">
+        <v>22</v>
+      </c>
+      <c r="I20">
+        <v>28</v>
+      </c>
+      <c r="J20">
+        <v>40</v>
+      </c>
+      <c r="K20">
+        <v>46</v>
+      </c>
+      <c r="L20">
+        <v>28</v>
+      </c>
+      <c r="M20">
+        <v>25</v>
+      </c>
+      <c r="N20">
+        <v>31</v>
+      </c>
+      <c r="O20" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="P20" s="25">
+        <f t="shared" si="1"/>
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
+        <v>20</v>
+      </c>
+      <c r="B21" s="26">
+        <v>45858</v>
+      </c>
+      <c r="C21" s="18">
+        <v>54</v>
+      </c>
+      <c r="D21">
+        <v>52</v>
+      </c>
+      <c r="E21">
+        <v>51</v>
+      </c>
+      <c r="F21">
+        <v>50</v>
+      </c>
+      <c r="G21">
+        <v>36</v>
+      </c>
+      <c r="H21">
+        <v>43</v>
+      </c>
+      <c r="I21">
+        <v>45</v>
+      </c>
+      <c r="J21">
+        <v>44</v>
+      </c>
+      <c r="K21">
+        <v>40</v>
+      </c>
+      <c r="L21">
+        <v>42</v>
+      </c>
+      <c r="O21" s="25">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="P21" s="25">
+        <f t="shared" si="1"/>
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>12</v>
+      </c>
+      <c r="B22" s="26">
+        <v>45859</v>
+      </c>
+      <c r="C22" s="18">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>31</v>
+      </c>
+      <c r="E22">
+        <v>27</v>
+      </c>
+      <c r="F22">
+        <v>21</v>
+      </c>
+      <c r="G22">
+        <v>24</v>
+      </c>
+      <c r="H22">
+        <v>31</v>
+      </c>
+      <c r="I22">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <v>28</v>
+      </c>
+      <c r="K22">
+        <v>19</v>
+      </c>
+      <c r="L22">
+        <v>17</v>
+      </c>
+      <c r="O22" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P22" s="25">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
+        <v>14</v>
+      </c>
+      <c r="B23" s="26">
+        <v>45860</v>
+      </c>
+      <c r="C23" s="18">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="O23" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P23" s="25">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>31</v>
+      </c>
+      <c r="B24" s="26">
+        <v>45861</v>
+      </c>
+      <c r="C24" s="18">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>9</v>
+      </c>
+      <c r="F24">
+        <v>14</v>
+      </c>
+      <c r="G24">
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>14</v>
+      </c>
+      <c r="I24">
+        <v>12</v>
+      </c>
+      <c r="J24">
+        <v>11</v>
+      </c>
+      <c r="K24">
+        <v>12</v>
+      </c>
+      <c r="L24">
+        <v>13</v>
+      </c>
+      <c r="O24" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P24" s="25">
+        <f t="shared" si="1"/>
+        <v>1.54</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="2"/>
+        <v>-19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
+        <v>24</v>
+      </c>
+      <c r="B25" s="26">
+        <v>45862</v>
+      </c>
+      <c r="C25" s="18">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>19</v>
+      </c>
+      <c r="I25">
+        <v>11</v>
+      </c>
+      <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25">
+        <v>13</v>
+      </c>
+      <c r="L25">
+        <v>11</v>
+      </c>
+      <c r="O25" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P25" s="25">
+        <f t="shared" si="1"/>
+        <v>2.96</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="2"/>
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>21</v>
+      </c>
+      <c r="B26" s="26">
+        <v>45863</v>
+      </c>
+      <c r="C26" s="18">
+        <v>16</v>
+      </c>
+      <c r="D26" s="18">
+        <v>12</v>
+      </c>
+      <c r="E26" s="18">
+        <v>15</v>
+      </c>
+      <c r="F26" s="18">
+        <v>21</v>
+      </c>
+      <c r="G26" s="18">
+        <v>17</v>
+      </c>
+      <c r="H26" s="22">
+        <v>16</v>
+      </c>
+      <c r="I26" s="18">
+        <v>18</v>
+      </c>
+      <c r="J26" s="18">
+        <v>18</v>
+      </c>
+      <c r="K26" s="18">
+        <v>19</v>
+      </c>
+      <c r="L26" s="18">
+        <v>14</v>
+      </c>
+      <c r="N26" s="19"/>
+      <c r="O26" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P26" s="25">
+        <f t="shared" si="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
+        <v>35</v>
+      </c>
+      <c r="B27" s="26">
+        <v>45864</v>
+      </c>
+      <c r="C27" s="18">
+        <v>24</v>
+      </c>
+      <c r="D27" s="18">
+        <v>23</v>
+      </c>
+      <c r="E27" s="18">
+        <v>21</v>
+      </c>
+      <c r="F27" s="18">
+        <v>25</v>
+      </c>
+      <c r="G27" s="18">
+        <v>21</v>
+      </c>
+      <c r="H27" s="22">
+        <v>23</v>
+      </c>
+      <c r="I27" s="18">
+        <v>21</v>
+      </c>
+      <c r="J27" s="18">
+        <v>21</v>
+      </c>
+      <c r="K27" s="18">
+        <v>20</v>
+      </c>
+      <c r="L27" s="18">
+        <v>21</v>
+      </c>
+      <c r="N27" s="19"/>
+      <c r="O27" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P27" s="25">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="2"/>
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>31</v>
+      </c>
+      <c r="B28" s="26">
+        <v>45865</v>
+      </c>
+      <c r="C28" s="18">
+        <v>13</v>
+      </c>
+      <c r="D28" s="18">
+        <v>18</v>
+      </c>
+      <c r="E28" s="18">
+        <v>17</v>
+      </c>
+      <c r="F28" s="18">
+        <v>13</v>
+      </c>
+      <c r="G28" s="18">
+        <v>16</v>
+      </c>
+      <c r="H28" s="22">
+        <v>16</v>
+      </c>
+      <c r="I28" s="18">
+        <v>13</v>
+      </c>
+      <c r="J28" s="18">
+        <v>18</v>
+      </c>
+      <c r="K28" s="18">
+        <v>16</v>
+      </c>
+      <c r="L28" s="18">
+        <v>17</v>
+      </c>
+      <c r="N28" s="19"/>
+      <c r="O28" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P28" s="25">
+        <f t="shared" si="1"/>
+        <v>1.67</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>11</v>
+      </c>
+      <c r="B29" s="26">
+        <v>45866</v>
+      </c>
+      <c r="C29" s="18">
+        <v>14</v>
+      </c>
+      <c r="D29" s="18">
+        <v>14</v>
+      </c>
+      <c r="E29" s="18">
+        <v>14</v>
+      </c>
+      <c r="F29" s="18">
+        <v>12</v>
+      </c>
+      <c r="G29" s="18">
+        <v>13</v>
+      </c>
+      <c r="H29" s="22">
+        <v>13</v>
+      </c>
+      <c r="I29" s="18">
+        <v>13</v>
+      </c>
+      <c r="J29" s="18">
+        <v>8</v>
+      </c>
+      <c r="K29" s="18">
+        <v>13</v>
+      </c>
+      <c r="L29" s="18">
+        <v>13</v>
+      </c>
+      <c r="N29" s="19"/>
+      <c r="O29" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="P29" s="25">
+        <f t="shared" si="1"/>
+        <v>1.62</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
+        <v>4</v>
+      </c>
+      <c r="B30" s="26">
+        <v>45867</v>
+      </c>
+      <c r="C30" s="18">
+        <v>16</v>
+      </c>
+      <c r="D30" s="18">
+        <v>13</v>
+      </c>
+      <c r="E30" s="18">
+        <v>18</v>
+      </c>
+      <c r="F30" s="18">
+        <v>17</v>
+      </c>
+      <c r="G30" s="18">
+        <v>12</v>
+      </c>
+      <c r="H30" s="22">
+        <v>18</v>
+      </c>
+      <c r="I30" s="18">
+        <v>13</v>
+      </c>
+      <c r="J30" s="18">
+        <v>13</v>
+      </c>
+      <c r="K30" s="18">
+        <v>15</v>
+      </c>
+      <c r="L30" s="18">
+        <v>15</v>
+      </c>
+      <c r="N30" s="19"/>
+      <c r="O30" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="P30" s="25">
+        <f t="shared" si="1"/>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>14</v>
+      </c>
+      <c r="B31" s="26">
+        <v>45868</v>
+      </c>
+      <c r="C31" s="18">
+        <v>9</v>
+      </c>
+      <c r="D31" s="18">
+        <v>7</v>
+      </c>
+      <c r="E31" s="18">
+        <v>10</v>
+      </c>
+      <c r="F31" s="18">
+        <v>10</v>
+      </c>
+      <c r="G31" s="18">
+        <v>8</v>
+      </c>
+      <c r="H31" s="22">
+        <v>6</v>
+      </c>
+      <c r="I31" s="18">
+        <v>10</v>
+      </c>
+      <c r="J31" s="18">
+        <v>10</v>
+      </c>
+      <c r="K31" s="18">
+        <v>8</v>
+      </c>
+      <c r="L31" s="18">
+        <v>9</v>
+      </c>
+      <c r="M31">
+        <v>8</v>
+      </c>
+      <c r="N31" s="19">
+        <v>10</v>
+      </c>
+      <c r="O31" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="P31" s="25">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
+        <v>41</v>
+      </c>
+      <c r="B32" s="26">
+        <v>45869</v>
+      </c>
+      <c r="C32" s="18">
+        <v>14</v>
+      </c>
+      <c r="D32" s="18">
+        <v>19</v>
+      </c>
+      <c r="E32" s="18">
+        <v>20</v>
+      </c>
+      <c r="F32" s="18">
+        <v>16</v>
+      </c>
+      <c r="G32" s="18">
+        <v>16</v>
+      </c>
+      <c r="H32" s="22">
+        <v>18</v>
+      </c>
+      <c r="I32" s="18">
+        <v>17</v>
+      </c>
+      <c r="J32" s="18">
+        <v>15</v>
+      </c>
+      <c r="K32" s="18">
+        <v>18</v>
+      </c>
+      <c r="L32" s="18">
+        <v>19</v>
+      </c>
+      <c r="M32">
+        <v>19</v>
+      </c>
+      <c r="N32" s="19">
+        <v>16</v>
+      </c>
+      <c r="O32" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P32" s="25">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="2"/>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>24</v>
+      </c>
+      <c r="B33" s="26">
+        <v>45870</v>
+      </c>
+      <c r="C33" s="18">
+        <v>35</v>
+      </c>
+      <c r="D33" s="18">
+        <v>32</v>
+      </c>
+      <c r="E33" s="18">
+        <v>30</v>
+      </c>
+      <c r="F33" s="18">
+        <v>34</v>
+      </c>
+      <c r="G33" s="18">
+        <v>25</v>
+      </c>
+      <c r="H33" s="22">
+        <v>33</v>
+      </c>
+      <c r="I33" s="18">
+        <v>33</v>
+      </c>
+      <c r="J33" s="18">
+        <v>31</v>
+      </c>
+      <c r="K33" s="18">
+        <v>33</v>
+      </c>
+      <c r="L33" s="18">
+        <v>28</v>
+      </c>
+      <c r="M33">
+        <v>36</v>
+      </c>
+      <c r="N33" s="19">
+        <v>37</v>
+      </c>
+      <c r="O33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="P33" s="25">
+        <f t="shared" si="1"/>
+        <v>3.14</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>87</v>
+      </c>
+      <c r="B34" s="26">
+        <v>45871</v>
+      </c>
+      <c r="C34" s="18">
+        <v>18</v>
+      </c>
+      <c r="D34" s="18">
+        <v>17</v>
+      </c>
+      <c r="E34" s="18">
+        <v>16</v>
+      </c>
+      <c r="F34" s="18">
+        <v>16</v>
+      </c>
+      <c r="G34" s="18">
+        <v>17</v>
+      </c>
+      <c r="H34" s="22">
+        <v>17</v>
+      </c>
+      <c r="I34" s="18">
+        <v>17</v>
+      </c>
+      <c r="J34" s="18">
+        <v>17</v>
+      </c>
+      <c r="K34" s="18">
+        <v>17</v>
+      </c>
+      <c r="L34" s="18">
+        <v>18</v>
+      </c>
+      <c r="M34">
+        <v>15</v>
+      </c>
+      <c r="N34" s="19">
+        <v>19</v>
+      </c>
+      <c r="O34" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P34" s="25">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="2"/>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="26">
+        <v>45872</v>
+      </c>
+      <c r="C35" s="18">
+        <v>38</v>
+      </c>
+      <c r="D35" s="18">
+        <v>55</v>
+      </c>
+      <c r="E35" s="18">
+        <v>39</v>
+      </c>
+      <c r="F35" s="18">
+        <v>54</v>
+      </c>
+      <c r="G35" s="18">
+        <v>49</v>
+      </c>
+      <c r="H35" s="22">
+        <v>46</v>
+      </c>
+      <c r="I35" s="18">
+        <v>51</v>
+      </c>
+      <c r="J35" s="18">
+        <v>40</v>
+      </c>
+      <c r="K35" s="18">
+        <v>57</v>
+      </c>
+      <c r="L35" s="18">
+        <v>38</v>
+      </c>
+      <c r="M35">
+        <v>35</v>
+      </c>
+      <c r="N35" s="19">
+        <v>41</v>
+      </c>
+      <c r="O35" s="25">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="P35" s="25">
+        <f t="shared" si="1"/>
+        <v>7.05</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36" s="26">
+        <v>45873</v>
+      </c>
+      <c r="C36" s="18">
+        <v>22</v>
+      </c>
+      <c r="D36" s="18">
+        <v>27</v>
+      </c>
+      <c r="E36" s="18">
+        <v>25</v>
+      </c>
+      <c r="F36" s="18">
+        <v>25</v>
+      </c>
+      <c r="G36" s="18">
+        <v>23</v>
+      </c>
+      <c r="H36" s="22">
+        <v>27</v>
+      </c>
+      <c r="I36" s="18">
+        <v>24</v>
+      </c>
+      <c r="J36" s="18">
+        <v>24</v>
+      </c>
+      <c r="K36" s="18">
+        <v>25</v>
+      </c>
+      <c r="L36" s="18">
+        <v>23</v>
+      </c>
+      <c r="M36">
+        <v>22</v>
+      </c>
+      <c r="N36" s="19">
+        <v>25</v>
+      </c>
+      <c r="O36" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="P36" s="25">
+        <f t="shared" si="1"/>
+        <v>1.44</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" s="26">
+        <v>45874</v>
+      </c>
+      <c r="C37" s="18">
+        <v>24</v>
+      </c>
+      <c r="D37" s="18">
+        <v>24</v>
+      </c>
+      <c r="E37" s="18">
+        <v>26</v>
+      </c>
+      <c r="F37" s="18">
+        <v>25</v>
+      </c>
+      <c r="G37" s="18">
+        <v>22</v>
+      </c>
+      <c r="H37" s="22">
+        <v>25</v>
+      </c>
+      <c r="I37" s="18">
+        <v>25</v>
+      </c>
+      <c r="J37" s="18">
+        <v>24</v>
+      </c>
+      <c r="K37" s="18">
+        <v>22</v>
+      </c>
+      <c r="L37" s="18">
+        <v>22</v>
+      </c>
+      <c r="M37">
+        <v>24</v>
+      </c>
+      <c r="N37" s="19">
+        <v>25</v>
+      </c>
+      <c r="O37" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="P37" s="25">
+        <f t="shared" si="1"/>
+        <v>1.29</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>23</v>
+      </c>
+      <c r="B38" s="26">
+        <v>45875</v>
+      </c>
+      <c r="C38" s="18">
+        <v>28</v>
+      </c>
+      <c r="D38" s="18">
+        <v>30</v>
+      </c>
+      <c r="E38" s="18">
+        <v>29</v>
+      </c>
+      <c r="F38" s="18">
+        <v>35</v>
+      </c>
+      <c r="G38" s="18">
+        <v>26</v>
+      </c>
+      <c r="H38" s="22">
+        <v>31</v>
+      </c>
+      <c r="I38" s="18">
+        <v>30</v>
+      </c>
+      <c r="J38" s="18">
+        <v>31</v>
+      </c>
+      <c r="K38" s="18">
+        <v>30</v>
+      </c>
+      <c r="L38" s="18">
+        <v>32</v>
+      </c>
+      <c r="M38">
+        <v>30</v>
+      </c>
+      <c r="N38" s="19">
+        <v>30</v>
+      </c>
+      <c r="O38" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P38" s="25">
+        <f t="shared" si="1"/>
+        <v>1.97</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>24</v>
+      </c>
+      <c r="B39" s="26">
+        <v>45876</v>
+      </c>
+      <c r="C39" s="18">
+        <v>27</v>
+      </c>
+      <c r="D39" s="18">
+        <v>28</v>
+      </c>
+      <c r="E39" s="18">
+        <v>28</v>
+      </c>
+      <c r="F39" s="18">
+        <v>24</v>
+      </c>
+      <c r="G39" s="18">
+        <v>28</v>
+      </c>
+      <c r="H39" s="22">
+        <v>27</v>
+      </c>
+      <c r="I39" s="18">
+        <v>23</v>
+      </c>
+      <c r="J39" s="18">
+        <v>26</v>
+      </c>
+      <c r="K39" s="18">
+        <v>26</v>
+      </c>
+      <c r="L39" s="18">
+        <v>28</v>
+      </c>
+      <c r="M39">
+        <v>26</v>
+      </c>
+      <c r="N39" s="19">
+        <v>26</v>
+      </c>
+      <c r="O39" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P39" s="25">
+        <f t="shared" si="1"/>
+        <v>1.55</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32</v>
+      </c>
+      <c r="B40" s="26">
+        <v>45877</v>
+      </c>
+      <c r="C40" s="18">
+        <v>20</v>
+      </c>
+      <c r="D40" s="18">
+        <v>18</v>
+      </c>
+      <c r="E40" s="18">
+        <v>22</v>
+      </c>
+      <c r="F40" s="18">
+        <v>21</v>
+      </c>
+      <c r="G40" s="18">
+        <v>24</v>
+      </c>
+      <c r="H40" s="22">
+        <v>24</v>
+      </c>
+      <c r="I40" s="18">
+        <v>17</v>
+      </c>
+      <c r="J40" s="18">
+        <v>22</v>
+      </c>
+      <c r="K40" s="18">
+        <v>19</v>
+      </c>
+      <c r="L40" s="18">
+        <v>21</v>
+      </c>
+      <c r="M40">
+        <v>21</v>
+      </c>
+      <c r="N40" s="19">
+        <v>23</v>
+      </c>
+      <c r="O40" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="P40" s="25">
+        <f t="shared" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>33</v>
+      </c>
+      <c r="B41" s="26">
+        <v>45878</v>
+      </c>
+      <c r="C41" s="18">
+        <v>14</v>
+      </c>
+      <c r="D41" s="18">
+        <v>15</v>
+      </c>
+      <c r="E41" s="18">
+        <v>14</v>
+      </c>
+      <c r="F41" s="18">
+        <v>19</v>
+      </c>
+      <c r="G41" s="18">
+        <v>16</v>
+      </c>
+      <c r="H41" s="22">
+        <v>19</v>
+      </c>
+      <c r="I41" s="18">
+        <v>20</v>
+      </c>
+      <c r="J41" s="18">
+        <v>16</v>
+      </c>
+      <c r="K41" s="18">
+        <v>14</v>
+      </c>
+      <c r="L41" s="18">
+        <v>14</v>
+      </c>
+      <c r="M41">
+        <v>24</v>
+      </c>
+      <c r="N41" s="19">
+        <v>19</v>
+      </c>
+      <c r="O41" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P41" s="25">
+        <f t="shared" si="1"/>
+        <v>2.92</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>52</v>
+      </c>
+      <c r="B42" s="26">
+        <v>45879</v>
+      </c>
+      <c r="C42" s="18">
+        <v>20</v>
+      </c>
+      <c r="D42" s="18">
+        <v>21</v>
+      </c>
+      <c r="E42" s="18">
+        <v>18</v>
+      </c>
+      <c r="F42" s="18">
+        <v>14</v>
+      </c>
+      <c r="G42" s="18">
+        <v>17</v>
+      </c>
+      <c r="H42" s="22">
+        <v>17</v>
+      </c>
+      <c r="I42" s="18">
+        <v>16</v>
+      </c>
+      <c r="J42" s="18">
+        <v>18</v>
+      </c>
+      <c r="K42" s="18">
+        <v>15</v>
+      </c>
+      <c r="L42" s="18">
+        <v>19</v>
+      </c>
+      <c r="M42">
+        <v>17</v>
+      </c>
+      <c r="N42" s="19">
+        <v>19</v>
+      </c>
+      <c r="O42" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="P42" s="25">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="2"/>
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>17</v>
+      </c>
+      <c r="B43" s="26">
+        <v>45880</v>
+      </c>
+      <c r="C43" s="18">
+        <v>23</v>
+      </c>
+      <c r="D43" s="18">
+        <v>22</v>
+      </c>
+      <c r="E43" s="18">
+        <v>19</v>
+      </c>
+      <c r="F43" s="18">
+        <v>19</v>
+      </c>
+      <c r="G43" s="18">
+        <v>20</v>
+      </c>
+      <c r="H43" s="22">
+        <v>16</v>
+      </c>
+      <c r="I43" s="18">
+        <v>20</v>
+      </c>
+      <c r="J43" s="18">
+        <v>17</v>
+      </c>
+      <c r="K43" s="18">
+        <v>20</v>
+      </c>
+      <c r="L43" s="18">
+        <v>24</v>
+      </c>
+      <c r="M43">
+        <v>18</v>
+      </c>
+      <c r="N43" s="19">
+        <v>20</v>
+      </c>
+      <c r="O43" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P43" s="25">
+        <f t="shared" si="1"/>
+        <v>2.02</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>11</v>
+      </c>
+      <c r="B44" s="26">
+        <v>45881</v>
+      </c>
+      <c r="C44" s="18">
+        <v>24</v>
+      </c>
+      <c r="D44" s="18">
+        <v>24</v>
+      </c>
+      <c r="E44" s="18">
+        <v>23</v>
+      </c>
+      <c r="F44" s="18">
+        <v>20</v>
+      </c>
+      <c r="G44" s="18">
+        <v>23</v>
+      </c>
+      <c r="H44" s="22">
+        <v>20</v>
+      </c>
+      <c r="I44" s="18">
+        <v>22</v>
+      </c>
+      <c r="J44" s="18">
+        <v>20</v>
+      </c>
+      <c r="K44" s="18">
+        <v>21</v>
+      </c>
+      <c r="L44" s="18">
+        <v>25</v>
+      </c>
+      <c r="M44">
+        <v>23</v>
+      </c>
+      <c r="N44" s="19">
+        <v>25</v>
+      </c>
+      <c r="O44" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P44" s="25">
+        <f t="shared" si="1"/>
+        <v>1.75</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>25</v>
+      </c>
+      <c r="B45" s="26">
+        <v>45882</v>
+      </c>
+      <c r="C45" s="27">
+        <v>22</v>
+      </c>
+      <c r="D45" s="20">
+        <v>23</v>
+      </c>
+      <c r="E45" s="20">
+        <v>21</v>
+      </c>
+      <c r="F45" s="20">
+        <v>26</v>
+      </c>
+      <c r="G45" s="20">
+        <v>22</v>
+      </c>
+      <c r="H45" s="23">
+        <v>24</v>
+      </c>
+      <c r="I45" s="20">
+        <v>23</v>
+      </c>
+      <c r="J45" s="20">
+        <v>22</v>
+      </c>
+      <c r="K45" s="20">
+        <v>22</v>
+      </c>
+      <c r="L45" s="20">
+        <v>22</v>
+      </c>
+      <c r="M45" s="20">
+        <v>22</v>
+      </c>
+      <c r="N45" s="21">
+        <v>27</v>
+      </c>
+      <c r="O45" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P45" s="25">
+        <f t="shared" si="1"/>
+        <v>1.71</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>36</v>
+      </c>
+      <c r="B46" s="26">
+        <v>45883</v>
+      </c>
+      <c r="C46">
+        <v>26</v>
+      </c>
+      <c r="D46">
+        <v>24</v>
+      </c>
+      <c r="E46">
+        <v>25</v>
+      </c>
+      <c r="F46">
+        <v>26</v>
+      </c>
+      <c r="G46">
+        <v>27</v>
+      </c>
+      <c r="H46">
+        <v>25</v>
+      </c>
+      <c r="I46">
+        <v>26</v>
+      </c>
+      <c r="J46">
+        <v>25</v>
+      </c>
+      <c r="K46">
+        <v>24</v>
+      </c>
+      <c r="L46">
+        <v>27</v>
+      </c>
+      <c r="M46">
+        <v>24</v>
+      </c>
+      <c r="N46">
+        <v>27</v>
+      </c>
+      <c r="O46" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P46" s="25">
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="26">
+        <v>45884</v>
+      </c>
+      <c r="C47">
+        <v>22</v>
+      </c>
+      <c r="O47" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P47" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="2"/>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>23</v>
+      </c>
+      <c r="B48" s="26">
+        <v>45885</v>
+      </c>
+      <c r="C48">
+        <v>19</v>
+      </c>
+      <c r="O48" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P48" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>58</v>
+      </c>
+      <c r="B49" s="26">
+        <v>45886</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+      <c r="O49" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="P49" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="2"/>
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50" s="26">
+        <v>45887</v>
+      </c>
+      <c r="C50">
+        <v>17</v>
+      </c>
+      <c r="O50" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P50" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>11</v>
+      </c>
+      <c r="B51" s="26">
+        <v>45888</v>
+      </c>
+      <c r="C51">
+        <v>19</v>
+      </c>
+      <c r="O51" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="P51" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52" s="26">
+        <v>45889</v>
+      </c>
+      <c r="C52">
+        <v>22</v>
+      </c>
+      <c r="O52" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="P52" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>10</v>
+      </c>
+      <c r="B53" s="26">
+        <v>45890</v>
+      </c>
+      <c r="C53">
+        <v>25</v>
+      </c>
+      <c r="O53" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P53" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>41</v>
+      </c>
+      <c r="B54" s="26">
+        <v>45891</v>
+      </c>
+      <c r="C54">
+        <v>27</v>
+      </c>
+      <c r="O54" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="P54" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>42</v>
+      </c>
+      <c r="B55" s="26">
+        <v>45892</v>
+      </c>
+      <c r="C55">
+        <v>18</v>
+      </c>
+      <c r="O55" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="P55" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="2"/>
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>78</v>
+      </c>
+      <c r="B56" s="26">
+        <v>45893</v>
+      </c>
+      <c r="C56">
+        <v>43</v>
+      </c>
+      <c r="O56" s="25">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="P56" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="2"/>
+        <v>-35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>11</v>
+      </c>
+      <c r="B57" s="26">
+        <v>45894</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="O57" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="P57" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>19</v>
+      </c>
+      <c r="B58" s="26">
+        <v>45895</v>
+      </c>
+      <c r="C58">
+        <v>26</v>
+      </c>
+      <c r="O58" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="P58" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>27</v>
+      </c>
+      <c r="B59" s="26">
+        <v>45896</v>
+      </c>
+      <c r="C59">
+        <v>28</v>
+      </c>
+      <c r="O59" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="P59" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>43</v>
+      </c>
+      <c r="B60" s="26">
+        <v>45897</v>
+      </c>
+      <c r="C60">
+        <v>25</v>
+      </c>
+      <c r="O60" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="P60" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>51</v>
+      </c>
+      <c r="B61" s="26">
+        <v>45898</v>
+      </c>
+      <c r="C61">
+        <v>23</v>
+      </c>
+      <c r="O61" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="P61" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="2"/>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>45</v>
+      </c>
+      <c r="B62" s="26">
+        <v>45899</v>
+      </c>
+      <c r="C62">
+        <v>17</v>
+      </c>
+      <c r="O62" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="P62" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="2"/>
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="26">
+        <v>45900</v>
+      </c>
+      <c r="C63">
+        <v>41</v>
+      </c>
+      <c r="O63" s="25">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="P63" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="2"/>
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" s="28"/>
+      <c r="B64" s="29">
+        <v>45901</v>
+      </c>
+      <c r="C64">
+        <v>35</v>
+      </c>
+      <c r="D64" s="28">
+        <v>18</v>
+      </c>
+      <c r="E64" s="28">
+        <v>26</v>
+      </c>
+      <c r="F64" s="28">
+        <v>26</v>
+      </c>
+      <c r="G64" s="28">
+        <v>26</v>
+      </c>
+      <c r="H64" s="28"/>
+      <c r="I64" s="28"/>
+      <c r="J64" s="28"/>
+      <c r="K64" s="28"/>
+      <c r="L64" s="28"/>
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+      <c r="O64" s="30">
+        <f>ROUND(AVERAGE(C64:N64),0)</f>
+        <v>26</v>
+      </c>
+      <c r="P64" s="30">
+        <f t="shared" si="1"/>
+        <v>3.2</v>
+      </c>
+      <c r="Q64" s="28"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B65" s="26">
+        <v>45902</v>
+      </c>
+      <c r="C65">
+        <v>33</v>
+      </c>
+      <c r="D65">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <v>23</v>
+      </c>
+      <c r="F65">
+        <v>34</v>
+      </c>
+      <c r="G65">
+        <v>36</v>
+      </c>
+      <c r="O65" s="25">
+        <f>ROUND(AVERAGE(C65:N65),0)</f>
+        <v>29</v>
+      </c>
+      <c r="P65" s="25">
+        <f t="shared" si="1"/>
+        <v>5.89</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B66" s="26">
+        <v>45903</v>
+      </c>
+      <c r="C66">
+        <v>19</v>
+      </c>
+      <c r="D66">
+        <v>18</v>
+      </c>
+      <c r="E66">
+        <v>19</v>
+      </c>
+      <c r="F66">
+        <v>21</v>
+      </c>
+      <c r="G66">
+        <v>28</v>
+      </c>
+      <c r="O66" s="25">
+        <f t="shared" ref="O66:O84" si="3">ROUND(AVERAGE(C66:N66),0)</f>
+        <v>21</v>
+      </c>
+      <c r="P66" s="25">
+        <f t="shared" ref="P66:P84" si="4">ROUND(_xlfn.STDEV.P(D66:O66),2)</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B67" s="26">
+        <v>45904</v>
+      </c>
+      <c r="C67">
+        <v>28</v>
+      </c>
+      <c r="D67">
+        <v>22</v>
+      </c>
+      <c r="E67">
+        <v>43</v>
+      </c>
+      <c r="F67">
+        <v>27</v>
+      </c>
+      <c r="G67">
+        <v>39</v>
+      </c>
+      <c r="O67" s="25">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="P67" s="25">
+        <f t="shared" si="4"/>
+        <v>7.66</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B68" s="26">
+        <v>45905</v>
+      </c>
+      <c r="C68">
+        <v>43</v>
+      </c>
+      <c r="D68">
+        <v>36</v>
+      </c>
+      <c r="E68">
+        <v>52</v>
+      </c>
+      <c r="F68">
+        <v>46</v>
+      </c>
+      <c r="G68">
+        <v>54</v>
+      </c>
+      <c r="O68" s="25">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="P68" s="25">
+        <f t="shared" si="4"/>
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B69" s="26">
+        <v>45906</v>
+      </c>
+      <c r="C69">
+        <v>52</v>
+      </c>
+      <c r="D69">
+        <v>54</v>
+      </c>
+      <c r="E69">
+        <v>53</v>
+      </c>
+      <c r="F69">
+        <v>47</v>
+      </c>
+      <c r="G69">
+        <v>50</v>
+      </c>
+      <c r="O69" s="25">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="P69" s="25">
+        <f t="shared" si="4"/>
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B70" s="26">
+        <v>45907</v>
+      </c>
+      <c r="C70">
+        <v>31</v>
+      </c>
+      <c r="D70">
+        <v>37</v>
+      </c>
+      <c r="E70">
+        <v>49</v>
+      </c>
+      <c r="F70">
+        <v>42</v>
+      </c>
+      <c r="G70">
+        <v>48</v>
+      </c>
+      <c r="O70" s="25">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="P70" s="25">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B71" s="26">
+        <v>45908</v>
+      </c>
+      <c r="C71">
+        <v>27</v>
+      </c>
+      <c r="D71">
+        <v>21</v>
+      </c>
+      <c r="E71">
+        <v>27</v>
+      </c>
+      <c r="F71">
+        <v>24</v>
+      </c>
+      <c r="G71">
+        <v>27</v>
+      </c>
+      <c r="O71" s="25">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="P71" s="25">
+        <f t="shared" si="4"/>
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B72" s="26">
+        <v>45909</v>
+      </c>
+      <c r="C72">
+        <v>24</v>
+      </c>
+      <c r="D72">
+        <v>22</v>
+      </c>
+      <c r="E72">
+        <v>26</v>
+      </c>
+      <c r="F72">
+        <v>27</v>
+      </c>
+      <c r="G72">
+        <v>28</v>
+      </c>
+      <c r="O72" s="25">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="P72" s="25">
+        <f t="shared" si="4"/>
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B73" s="26">
+        <v>45910</v>
+      </c>
+      <c r="C73">
+        <v>21</v>
+      </c>
+      <c r="D73">
+        <v>24</v>
+      </c>
+      <c r="E73">
+        <v>36</v>
+      </c>
+      <c r="F73">
+        <v>27</v>
+      </c>
+      <c r="G73">
+        <v>27</v>
+      </c>
+      <c r="O73" s="25">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="P73" s="25">
+        <f t="shared" si="4"/>
+        <v>4.07</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B74" s="26">
+        <v>45911</v>
+      </c>
+      <c r="C74">
+        <v>24</v>
+      </c>
+      <c r="D74">
+        <v>29</v>
+      </c>
+      <c r="E74">
+        <v>33</v>
+      </c>
+      <c r="F74">
+        <v>35</v>
+      </c>
+      <c r="G74">
+        <v>37</v>
+      </c>
+      <c r="O74" s="25">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="P74" s="25">
+        <f t="shared" si="4"/>
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B75" s="26">
+        <v>45912</v>
+      </c>
+      <c r="C75">
+        <v>27</v>
+      </c>
+      <c r="D75">
+        <v>19</v>
+      </c>
+      <c r="E75">
+        <v>31</v>
+      </c>
+      <c r="F75">
+        <v>37</v>
+      </c>
+      <c r="G75">
+        <v>32</v>
+      </c>
+      <c r="O75" s="25">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="P75" s="25">
+        <f t="shared" si="4"/>
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B76" s="26">
+        <v>45913</v>
+      </c>
+      <c r="C76">
+        <v>34</v>
+      </c>
+      <c r="D76">
+        <v>48</v>
+      </c>
+      <c r="E76">
+        <v>49</v>
+      </c>
+      <c r="F76">
+        <v>46</v>
+      </c>
+      <c r="G76">
+        <v>37</v>
+      </c>
+      <c r="O76" s="25">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="P76" s="25">
+        <f t="shared" si="4"/>
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B77" s="26">
+        <v>45914</v>
+      </c>
+      <c r="C77">
+        <v>42</v>
+      </c>
+      <c r="D77">
+        <v>23</v>
+      </c>
+      <c r="E77">
+        <v>46</v>
+      </c>
+      <c r="F77">
+        <v>68</v>
+      </c>
+      <c r="G77">
+        <v>80</v>
+      </c>
+      <c r="O77" s="25">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="P77" s="25">
+        <f t="shared" si="4"/>
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B78" s="26">
+        <v>45915</v>
+      </c>
+      <c r="C78">
+        <v>25</v>
+      </c>
+      <c r="D78">
+        <v>25</v>
+      </c>
+      <c r="E78">
+        <v>23</v>
+      </c>
+      <c r="F78">
+        <v>20</v>
+      </c>
+      <c r="G78">
+        <v>19</v>
+      </c>
+      <c r="O78" s="25">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="P78" s="25">
+        <f t="shared" si="4"/>
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B79" s="26">
+        <v>45916</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79">
+        <v>28</v>
+      </c>
+      <c r="E79">
+        <v>33</v>
+      </c>
+      <c r="F79">
+        <v>34</v>
+      </c>
+      <c r="G79">
+        <v>32</v>
+      </c>
+      <c r="O79" s="25">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="P79" s="25">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B80" s="26">
+        <v>45917</v>
+      </c>
+      <c r="C80">
+        <v>23</v>
+      </c>
+      <c r="D80">
+        <v>25</v>
+      </c>
+      <c r="E80">
+        <v>37</v>
+      </c>
+      <c r="F80">
+        <v>22</v>
+      </c>
+      <c r="G80">
+        <v>27</v>
+      </c>
+      <c r="O80" s="25">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="P80" s="25">
+        <f t="shared" si="4"/>
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B81" s="26">
+        <v>45918</v>
+      </c>
+      <c r="C81" s="34">
+        <v>18</v>
+      </c>
+      <c r="D81">
+        <v>27</v>
+      </c>
+      <c r="E81">
+        <v>28</v>
+      </c>
+      <c r="F81">
+        <v>29</v>
+      </c>
+      <c r="G81">
+        <v>35</v>
+      </c>
+      <c r="O81" s="25">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="P81" s="25">
+        <f t="shared" si="4"/>
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B82" s="26">
+        <v>45919</v>
+      </c>
+      <c r="C82" s="18">
+        <v>36</v>
+      </c>
+      <c r="D82">
+        <v>32</v>
+      </c>
+      <c r="E82">
+        <v>47</v>
+      </c>
+      <c r="F82">
+        <v>30</v>
+      </c>
+      <c r="G82">
+        <v>35</v>
+      </c>
+      <c r="O82" s="25">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="P82" s="25">
+        <f t="shared" si="4"/>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="33" t="s">
+        <v>41</v>
       </c>
       <c r="D83" s="34"/>
       <c r="E83" s="34"/>
@@ -18588,21 +22376,18 @@
       <c r="L83" s="34"/>
       <c r="M83" s="34"/>
       <c r="N83" s="35"/>
-      <c r="O83" s="36">
+      <c r="O83" s="36" t="e">
         <f>ROUND(AVERAGE(C83:N83),2)</f>
-        <v>24.96</v>
-      </c>
-      <c r="P83" s="36">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P83" s="36" t="e">
         <f>ROUND(_xlfn.STDEV.P(D83:O83),2)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="84" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B84" s="22" t="s">
         <v>42</v>
-      </c>
-      <c r="C84" s="18">
-        <v>15.64</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="18"/>
@@ -18615,20 +22400,20 @@
       <c r="L84" s="18"/>
       <c r="M84" s="18"/>
       <c r="N84" s="19"/>
-      <c r="O84" s="25">
+      <c r="O84" s="25" t="e">
         <f>ROUND(AVERAGE(C84:N84),2)</f>
-        <v>15.64</v>
-      </c>
-      <c r="P84" s="25">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P84" s="25" t="e">
         <f>ROUND(_xlfn.STDEV.P(D84:O84),2)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:N1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C83:L83 N83">
+  <conditionalFormatting sqref="D83:L83 C81 N83">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q63">

</xml_diff>

<commit_message>
updated data, finetuned model param, updated notes
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data/mornings.xlsx
+++ b/restaurant_analytics/data/mornings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DBD47BF-18EE-4B77-9E39-207D023351D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8140A7-9AAF-4930-AF77-A94ADBB344A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>day</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>actual</t>
+  </si>
+  <si>
+    <t>diwali</t>
+  </si>
+  <si>
+    <t>halloween</t>
   </si>
 </sst>
 </file>
@@ -436,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -517,6 +523,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -886,11 +895,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K553"/>
+  <dimension ref="A1:K604"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A515" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D534" sqref="D534"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A570" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I601" sqref="I601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14875,7 +14884,7 @@
         <v>0</v>
       </c>
       <c r="E530" s="11">
-        <v>68.7</v>
+        <v>67.8</v>
       </c>
       <c r="F530" s="11">
         <v>0</v>
@@ -14884,7 +14893,7 @@
         <v>0</v>
       </c>
       <c r="H530" s="11">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I530" s="10" t="s">
         <v>19</v>
@@ -14904,7 +14913,7 @@
         <v>13</v>
       </c>
       <c r="E531" s="11">
-        <v>70.3</v>
+        <v>69.8</v>
       </c>
       <c r="F531" s="11">
         <v>0</v>
@@ -14913,11 +14922,10 @@
         <v>0</v>
       </c>
       <c r="H531" s="11">
-        <v>4.2</v>
-      </c>
-      <c r="J531" s="37">
-        <v>5.4949999999999992</v>
-      </c>
+        <v>3.2</v>
+      </c>
+      <c r="I531" s="38"/>
+      <c r="J531" s="37"/>
     </row>
     <row r="532" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A532" s="7">
@@ -14933,20 +14941,19 @@
         <v>12</v>
       </c>
       <c r="E532" s="11">
-        <v>66.900000000000006</v>
+        <v>65.5</v>
       </c>
       <c r="F532" s="11">
-        <v>0.52800000000000002</v>
+        <v>0.217</v>
       </c>
       <c r="G532" s="11">
         <v>0</v>
       </c>
       <c r="H532" s="11">
-        <v>10.4</v>
-      </c>
-      <c r="J532" s="37">
-        <v>3.0949999999999998</v>
-      </c>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I532" s="38"/>
+      <c r="J532" s="37"/>
     </row>
     <row r="533" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A533" s="7">
@@ -14962,7 +14969,7 @@
         <v>19</v>
       </c>
       <c r="E533" s="11">
-        <v>60.6</v>
+        <v>58.3</v>
       </c>
       <c r="F533" s="11">
         <v>0</v>
@@ -14971,11 +14978,10 @@
         <v>0</v>
       </c>
       <c r="H533" s="11">
-        <v>9.9</v>
-      </c>
-      <c r="J533" s="37">
-        <v>5.6</v>
-      </c>
+        <v>8.6</v>
+      </c>
+      <c r="I533" s="38"/>
+      <c r="J533" s="37"/>
     </row>
     <row r="534" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A534" s="7">
@@ -14988,23 +14994,22 @@
         <v>45905</v>
       </c>
       <c r="D534" s="16">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E534" s="11">
-        <v>61</v>
+        <v>61.2</v>
       </c>
       <c r="F534" s="11">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="G534" s="11">
         <v>0</v>
       </c>
       <c r="H534" s="11">
-        <v>12.2</v>
-      </c>
-      <c r="J534" s="37">
-        <v>3.9899999999999998</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I534" s="38"/>
+      <c r="J534" s="37"/>
     </row>
     <row r="535" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A535" s="7">
@@ -15017,10 +15022,10 @@
         <v>45906</v>
       </c>
       <c r="D535" s="16">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E535" s="11">
-        <v>59.7</v>
+        <v>57.2</v>
       </c>
       <c r="F535" s="11">
         <v>0</v>
@@ -15029,11 +15034,10 @@
         <v>0</v>
       </c>
       <c r="H535" s="11">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J535" s="37">
-        <v>4.7050000000000001</v>
-      </c>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I535" s="38"/>
+      <c r="J535" s="37"/>
     </row>
     <row r="536" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A536" s="7">
@@ -15046,23 +15050,22 @@
         <v>45907</v>
       </c>
       <c r="D536" s="16">
-        <v>36.5</v>
+        <v>51</v>
       </c>
       <c r="E536" s="11">
-        <v>60.6</v>
+        <v>57.9</v>
       </c>
       <c r="F536" s="11">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="G536" s="11">
         <v>0</v>
       </c>
       <c r="H536" s="11">
-        <v>7.3</v>
-      </c>
-      <c r="J536" s="37">
-        <v>3.4649999999999999</v>
-      </c>
+        <v>6.2</v>
+      </c>
+      <c r="I536" s="38"/>
+      <c r="J536" s="37"/>
     </row>
     <row r="537" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A537" s="7">
@@ -15075,23 +15078,22 @@
         <v>45908</v>
       </c>
       <c r="D537" s="16">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E537" s="11">
-        <v>62.6</v>
+        <v>61.5</v>
       </c>
       <c r="F537" s="11">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="G537" s="11">
         <v>0</v>
       </c>
       <c r="H537" s="11">
-        <v>6.4</v>
-      </c>
-      <c r="J537" s="37">
-        <v>2.98</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I537" s="38"/>
+      <c r="J537" s="37"/>
     </row>
     <row r="538" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A538" s="7">
@@ -15104,10 +15106,10 @@
         <v>45909</v>
       </c>
       <c r="D538" s="16">
-        <v>23.5</v>
+        <v>29</v>
       </c>
       <c r="E538" s="11">
-        <v>65.3</v>
+        <v>64.8</v>
       </c>
       <c r="F538" s="11">
         <v>0</v>
@@ -15116,11 +15118,10 @@
         <v>0</v>
       </c>
       <c r="H538" s="11">
-        <v>7.5</v>
-      </c>
-      <c r="J538" s="37">
-        <v>2.1749999999999998</v>
-      </c>
+        <v>6.2</v>
+      </c>
+      <c r="I538" s="38"/>
+      <c r="J538" s="37"/>
     </row>
     <row r="539" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A539" s="7">
@@ -15133,10 +15134,10 @@
         <v>45910</v>
       </c>
       <c r="D539" s="16">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E539" s="11">
-        <v>66.900000000000006</v>
+        <v>70.7</v>
       </c>
       <c r="F539" s="11">
         <v>0</v>
@@ -15145,11 +15146,10 @@
         <v>0</v>
       </c>
       <c r="H539" s="11">
-        <v>8</v>
-      </c>
-      <c r="J539" s="37">
-        <v>3.2949999999999999</v>
-      </c>
+        <v>5.2</v>
+      </c>
+      <c r="I539" s="38"/>
+      <c r="J539" s="37"/>
     </row>
     <row r="540" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A540" s="7">
@@ -15162,10 +15162,10 @@
         <v>45911</v>
       </c>
       <c r="D540" s="16">
-        <v>29.5</v>
+        <v>41</v>
       </c>
       <c r="E540" s="11">
-        <v>69</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="F540" s="11">
         <v>0</v>
@@ -15174,11 +15174,10 @@
         <v>0</v>
       </c>
       <c r="H540" s="11">
-        <v>6</v>
-      </c>
-      <c r="J540" s="37">
-        <v>2.33</v>
-      </c>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I540" s="38"/>
+      <c r="J540" s="37"/>
     </row>
     <row r="541" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A541" s="7">
@@ -15191,23 +15190,22 @@
         <v>45912</v>
       </c>
       <c r="D541" s="16">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E541" s="11">
-        <v>70</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="F541" s="11">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="G541" s="11">
         <v>0</v>
       </c>
       <c r="H541" s="11">
-        <v>4</v>
-      </c>
-      <c r="J541" s="37">
-        <v>4.0549999999999997</v>
-      </c>
+        <v>6.5</v>
+      </c>
+      <c r="I541" s="38"/>
+      <c r="J541" s="37"/>
     </row>
     <row r="542" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A542" s="7">
@@ -15220,23 +15218,22 @@
         <v>45913</v>
       </c>
       <c r="D542" s="16">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E542" s="11">
-        <v>69</v>
+        <v>71.2</v>
       </c>
       <c r="F542" s="11">
-        <v>0</v>
+        <v>0.58299999999999996</v>
       </c>
       <c r="G542" s="11">
         <v>0</v>
       </c>
       <c r="H542" s="11">
-        <v>8</v>
-      </c>
-      <c r="J542" s="37">
-        <v>4.9399999999999995</v>
-      </c>
+        <v>8.6</v>
+      </c>
+      <c r="I542" s="38"/>
+      <c r="J542" s="37"/>
     </row>
     <row r="543" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A543" s="7">
@@ -15249,23 +15246,22 @@
         <v>45914</v>
       </c>
       <c r="D543" s="16">
-        <v>48.5</v>
+        <v>41</v>
       </c>
       <c r="E543" s="11">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F543" s="11">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="G543" s="11">
         <v>0</v>
       </c>
       <c r="H543" s="11">
-        <v>4</v>
-      </c>
-      <c r="J543" s="37">
-        <v>15.91</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="I543" s="38"/>
+      <c r="J543" s="37"/>
     </row>
     <row r="544" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A544" s="7">
@@ -15278,10 +15274,10 @@
         <v>45915</v>
       </c>
       <c r="D544" s="16">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E544" s="11">
-        <v>56.5</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="F544" s="11">
         <v>0</v>
@@ -15290,11 +15286,10 @@
         <v>0</v>
       </c>
       <c r="H544" s="11">
-        <v>10</v>
-      </c>
-      <c r="J544" s="37">
-        <v>3.6150000000000002</v>
-      </c>
+        <v>6.8</v>
+      </c>
+      <c r="I544" s="38"/>
+      <c r="J544" s="37"/>
     </row>
     <row r="545" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A545" s="7">
@@ -15307,10 +15302,10 @@
         <v>45916</v>
       </c>
       <c r="D545" s="16">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E545" s="11">
-        <v>57</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="F545" s="11">
         <v>0</v>
@@ -15319,11 +15314,10 @@
         <v>0</v>
       </c>
       <c r="H545" s="11">
-        <v>2</v>
-      </c>
-      <c r="J545" s="37">
-        <v>4.03</v>
-      </c>
+        <v>4.3</v>
+      </c>
+      <c r="I545" s="38"/>
+      <c r="J545" s="37"/>
     </row>
     <row r="546" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A546" s="7">
@@ -15336,23 +15330,22 @@
         <v>45917</v>
       </c>
       <c r="D546" s="16">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E546" s="11">
-        <v>58.5</v>
+        <v>72</v>
       </c>
       <c r="F546" s="11">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="G546" s="11">
         <v>0</v>
       </c>
       <c r="H546" s="11">
-        <v>5</v>
-      </c>
-      <c r="J546" s="37">
-        <v>4.57</v>
-      </c>
+        <v>4.5</v>
+      </c>
+      <c r="I546" s="38"/>
+      <c r="J546" s="37"/>
     </row>
     <row r="547" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A547" s="7">
@@ -15365,23 +15358,22 @@
         <v>45918</v>
       </c>
       <c r="D547" s="16">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E547" s="11">
-        <v>59.5</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="F547" s="11">
-        <v>0.56000000000000005</v>
+        <v>0</v>
       </c>
       <c r="G547" s="11">
         <v>0</v>
       </c>
       <c r="H547" s="11">
-        <v>8</v>
-      </c>
-      <c r="J547" s="37">
-        <v>2.9950000000000001</v>
-      </c>
+        <v>3.5</v>
+      </c>
+      <c r="I547" s="38"/>
+      <c r="J547" s="37"/>
     </row>
     <row r="548" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A548" s="7">
@@ -15394,43 +15386,1412 @@
         <v>45919</v>
       </c>
       <c r="D548" s="16">
-        <v>31.5</v>
+        <v>37</v>
       </c>
       <c r="E548" s="11">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F548" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G548" s="11">
+        <v>0</v>
+      </c>
+      <c r="H548" s="11">
+        <v>5.2</v>
+      </c>
+      <c r="I548" s="38"/>
+      <c r="J548" s="37"/>
+    </row>
+    <row r="549" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A549" s="7">
+        <v>7</v>
+      </c>
+      <c r="B549" s="7">
+        <v>548</v>
+      </c>
+      <c r="C549" s="8">
+        <v>45920</v>
+      </c>
+      <c r="D549" s="16">
+        <v>22</v>
+      </c>
+      <c r="E549" s="11">
+        <v>70.7</v>
+      </c>
+      <c r="F549" s="11">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="G549" s="11">
+        <v>0</v>
+      </c>
+      <c r="H549" s="11">
+        <v>5</v>
+      </c>
+      <c r="I549" s="38"/>
+    </row>
+    <row r="550" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A550" s="7">
+        <v>1</v>
+      </c>
+      <c r="B550" s="7">
+        <v>549</v>
+      </c>
+      <c r="C550" s="8">
+        <v>45921</v>
+      </c>
+      <c r="D550" s="16">
+        <v>24</v>
+      </c>
+      <c r="E550" s="11">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F550" s="11">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="G550" s="11">
+        <v>0</v>
+      </c>
+      <c r="H550" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="I550" s="38"/>
+    </row>
+    <row r="551" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A551" s="7">
+        <v>2</v>
+      </c>
+      <c r="B551" s="7">
+        <v>550</v>
+      </c>
+      <c r="C551" s="8">
+        <v>45922</v>
+      </c>
+      <c r="D551" s="16">
+        <v>12</v>
+      </c>
+      <c r="E551" s="11">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="F551" s="11">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G551" s="11">
+        <v>0</v>
+      </c>
+      <c r="H551" s="11">
+        <v>7.2</v>
+      </c>
+      <c r="I551" s="38"/>
+    </row>
+    <row r="552" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A552" s="7">
+        <v>3</v>
+      </c>
+      <c r="B552" s="7">
+        <v>551</v>
+      </c>
+      <c r="C552" s="8">
+        <v>45923</v>
+      </c>
+      <c r="D552" s="16">
+        <v>11</v>
+      </c>
+      <c r="E552" s="11">
+        <v>69.8</v>
+      </c>
+      <c r="F552" s="11">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G552" s="11">
+        <v>0</v>
+      </c>
+      <c r="H552" s="11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I552" s="38"/>
+    </row>
+    <row r="553" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A553" s="7">
+        <v>4</v>
+      </c>
+      <c r="B553" s="7">
+        <v>552</v>
+      </c>
+      <c r="C553" s="8">
+        <v>45924</v>
+      </c>
+      <c r="D553" s="16">
+        <v>33</v>
+      </c>
+      <c r="E553" s="11">
+        <v>65.8</v>
+      </c>
+      <c r="F553" s="11">
+        <v>0</v>
+      </c>
+      <c r="G553" s="11">
+        <v>0</v>
+      </c>
+      <c r="H553" s="11">
+        <v>11.5</v>
+      </c>
+      <c r="I553" s="38"/>
+    </row>
+    <row r="554" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A554" s="7">
+        <v>5</v>
+      </c>
+      <c r="B554" s="7">
+        <v>553</v>
+      </c>
+      <c r="C554" s="8">
+        <v>45925</v>
+      </c>
+      <c r="D554" s="16">
+        <v>21</v>
+      </c>
+      <c r="E554" s="11">
+        <v>65.8</v>
+      </c>
+      <c r="F554" s="11">
+        <v>0</v>
+      </c>
+      <c r="G554" s="11">
+        <v>0</v>
+      </c>
+      <c r="H554" s="11">
+        <v>6.7</v>
+      </c>
+      <c r="I554" s="38"/>
+    </row>
+    <row r="555" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A555" s="7">
+        <v>6</v>
+      </c>
+      <c r="B555" s="7">
+        <v>554</v>
+      </c>
+      <c r="C555" s="8">
+        <v>45926</v>
+      </c>
+      <c r="D555" s="16">
+        <v>27</v>
+      </c>
+      <c r="E555" s="11">
+        <v>70.3</v>
+      </c>
+      <c r="F555" s="11">
+        <v>0</v>
+      </c>
+      <c r="G555" s="11">
+        <v>0</v>
+      </c>
+      <c r="H555" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="I555" s="38"/>
+    </row>
+    <row r="556" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A556" s="7">
+        <v>7</v>
+      </c>
+      <c r="B556" s="7">
+        <v>555</v>
+      </c>
+      <c r="C556" s="8">
+        <v>45927</v>
+      </c>
+      <c r="D556" s="16">
+        <v>37</v>
+      </c>
+      <c r="E556" s="11">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="F556" s="11">
+        <v>0</v>
+      </c>
+      <c r="G556" s="11">
+        <v>0</v>
+      </c>
+      <c r="H556" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="I556" s="38"/>
+    </row>
+    <row r="557" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A557" s="7">
+        <v>1</v>
+      </c>
+      <c r="B557" s="7">
+        <v>556</v>
+      </c>
+      <c r="C557" s="8">
+        <v>45928</v>
+      </c>
+      <c r="D557" s="16">
+        <v>58</v>
+      </c>
+      <c r="E557" s="11">
+        <v>70.7</v>
+      </c>
+      <c r="F557" s="11">
+        <v>0</v>
+      </c>
+      <c r="G557" s="11">
+        <v>0</v>
+      </c>
+      <c r="H557" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="I557" s="38"/>
+    </row>
+    <row r="558" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A558" s="7">
+        <v>2</v>
+      </c>
+      <c r="B558" s="7">
+        <v>557</v>
+      </c>
+      <c r="C558" s="8">
+        <v>45929</v>
+      </c>
+      <c r="D558" s="16">
+        <v>16</v>
+      </c>
+      <c r="E558" s="11">
+        <v>73.8</v>
+      </c>
+      <c r="F558" s="11">
+        <v>0</v>
+      </c>
+      <c r="G558" s="11">
+        <v>0</v>
+      </c>
+      <c r="H558" s="11">
+        <v>3.3</v>
+      </c>
+      <c r="I558" s="38"/>
+    </row>
+    <row r="559" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A559" s="7">
+        <v>3</v>
+      </c>
+      <c r="B559" s="7">
+        <v>558</v>
+      </c>
+      <c r="C559" s="8">
+        <v>45930</v>
+      </c>
+      <c r="D559" s="16">
+        <v>18</v>
+      </c>
+      <c r="E559" s="11">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="F559" s="11">
+        <v>0</v>
+      </c>
+      <c r="G559" s="11">
+        <v>0</v>
+      </c>
+      <c r="H559" s="11">
+        <v>6.6</v>
+      </c>
+      <c r="I559" s="38"/>
+    </row>
+    <row r="560" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A560" s="7">
+        <v>4</v>
+      </c>
+      <c r="B560" s="7">
+        <v>559</v>
+      </c>
+      <c r="C560" s="8">
+        <v>45931</v>
+      </c>
+      <c r="D560" s="16">
+        <v>23</v>
+      </c>
+      <c r="E560" s="11">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="F560" s="11">
+        <v>0</v>
+      </c>
+      <c r="G560" s="11">
+        <v>0</v>
+      </c>
+      <c r="H560" s="11">
+        <v>8.6</v>
+      </c>
+      <c r="I560" s="38"/>
+    </row>
+    <row r="561" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A561" s="7">
+        <v>5</v>
+      </c>
+      <c r="B561" s="7">
+        <v>560</v>
+      </c>
+      <c r="C561" s="8">
+        <v>45932</v>
+      </c>
+      <c r="D561" s="16">
+        <v>23</v>
+      </c>
+      <c r="E561" s="11">
+        <v>70.5</v>
+      </c>
+      <c r="F561" s="11">
+        <v>0</v>
+      </c>
+      <c r="G561" s="11">
+        <v>0</v>
+      </c>
+      <c r="H561" s="11">
+        <v>6</v>
+      </c>
+      <c r="I561" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="562" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A562" s="7">
+        <v>6</v>
+      </c>
+      <c r="B562" s="7">
+        <v>561</v>
+      </c>
+      <c r="C562" s="8">
+        <v>45933</v>
+      </c>
+      <c r="D562" s="16">
+        <v>34</v>
+      </c>
+      <c r="E562" s="11">
+        <v>76.3</v>
+      </c>
+      <c r="F562" s="11">
+        <v>0</v>
+      </c>
+      <c r="G562" s="11">
+        <v>0</v>
+      </c>
+      <c r="H562" s="11">
+        <v>5.4</v>
+      </c>
+      <c r="I562" s="38"/>
+    </row>
+    <row r="563" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A563" s="7">
+        <v>7</v>
+      </c>
+      <c r="B563" s="7">
+        <v>562</v>
+      </c>
+      <c r="C563" s="8">
+        <v>45934</v>
+      </c>
+      <c r="D563" s="16">
+        <v>42</v>
+      </c>
+      <c r="E563" s="11">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="F563" s="11">
+        <v>0</v>
+      </c>
+      <c r="G563" s="11">
+        <v>0</v>
+      </c>
+      <c r="H563" s="11">
+        <v>7.8</v>
+      </c>
+      <c r="I563" s="38"/>
+    </row>
+    <row r="564" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A564" s="7">
+        <v>1</v>
+      </c>
+      <c r="B564" s="7">
+        <v>563</v>
+      </c>
+      <c r="C564" s="8">
+        <v>45935</v>
+      </c>
+      <c r="D564" s="16">
+        <v>50</v>
+      </c>
+      <c r="E564" s="11">
+        <v>75</v>
+      </c>
+      <c r="F564" s="11">
+        <v>0</v>
+      </c>
+      <c r="G564" s="11">
+        <v>0</v>
+      </c>
+      <c r="H564" s="11">
+        <v>10.6</v>
+      </c>
+      <c r="I564" s="38"/>
+    </row>
+    <row r="565" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A565" s="7">
+        <v>2</v>
+      </c>
+      <c r="B565" s="7">
+        <v>564</v>
+      </c>
+      <c r="C565" s="8">
+        <v>45936</v>
+      </c>
+      <c r="D565" s="16">
+        <v>25</v>
+      </c>
+      <c r="E565" s="11">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="F565" s="11">
+        <v>0.441</v>
+      </c>
+      <c r="G565" s="11">
+        <v>0</v>
+      </c>
+      <c r="H565" s="11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I565" s="38"/>
+    </row>
+    <row r="566" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A566" s="7">
+        <v>3</v>
+      </c>
+      <c r="B566" s="7">
+        <v>565</v>
+      </c>
+      <c r="C566" s="8">
+        <v>45937</v>
+      </c>
+      <c r="E566" s="11">
+        <v>61.2</v>
+      </c>
+      <c r="F566" s="11">
+        <v>0.48</v>
+      </c>
+      <c r="G566" s="11">
+        <v>0</v>
+      </c>
+      <c r="H566" s="11">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I566" s="38"/>
+    </row>
+    <row r="567" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A567" s="7">
+        <v>4</v>
+      </c>
+      <c r="B567" s="7">
+        <v>566</v>
+      </c>
+      <c r="C567" s="8">
+        <v>45938</v>
+      </c>
+      <c r="E567" s="11">
+        <v>57.9</v>
+      </c>
+      <c r="F567" s="11">
+        <v>0</v>
+      </c>
+      <c r="G567" s="11">
+        <v>0</v>
+      </c>
+      <c r="H567" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="I567" s="38"/>
+    </row>
+    <row r="568" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A568" s="7">
+        <v>5</v>
+      </c>
+      <c r="B568" s="7">
+        <v>567</v>
+      </c>
+      <c r="C568" s="8">
+        <v>45939</v>
+      </c>
+      <c r="E568" s="11">
+        <v>59.5</v>
+      </c>
+      <c r="F568" s="11">
+        <v>0.18</v>
+      </c>
+      <c r="G568" s="11">
+        <v>0</v>
+      </c>
+      <c r="H568" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="I568" s="38"/>
+    </row>
+    <row r="569" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A569" s="7">
+        <v>6</v>
+      </c>
+      <c r="B569" s="7">
+        <v>568</v>
+      </c>
+      <c r="C569" s="8">
+        <v>45940</v>
+      </c>
+      <c r="E569" s="11">
+        <v>61.9</v>
+      </c>
+      <c r="F569" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="G569" s="11">
+        <v>0</v>
+      </c>
+      <c r="H569" s="11">
+        <v>9.1</v>
+      </c>
+      <c r="I569" s="38"/>
+    </row>
+    <row r="570" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A570" s="7">
+        <v>7</v>
+      </c>
+      <c r="B570" s="7">
+        <v>569</v>
+      </c>
+      <c r="C570" s="8">
+        <v>45941</v>
+      </c>
+      <c r="E570" s="11">
+        <v>59.9</v>
+      </c>
+      <c r="F570" s="11">
+        <v>0</v>
+      </c>
+      <c r="G570" s="11">
+        <v>0</v>
+      </c>
+      <c r="H570" s="11">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I570" s="38"/>
+    </row>
+    <row r="571" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A571" s="7">
+        <v>1</v>
+      </c>
+      <c r="B571" s="7">
+        <v>570</v>
+      </c>
+      <c r="C571" s="8">
+        <v>45942</v>
+      </c>
+      <c r="E571" s="11">
+        <v>59.4</v>
+      </c>
+      <c r="F571" s="11">
+        <v>0</v>
+      </c>
+      <c r="G571" s="11">
+        <v>0</v>
+      </c>
+      <c r="H571" s="11">
+        <v>7.9</v>
+      </c>
+      <c r="I571" s="38"/>
+    </row>
+    <row r="572" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A572" s="7">
+        <v>2</v>
+      </c>
+      <c r="B572" s="7">
+        <v>571</v>
+      </c>
+      <c r="C572" s="8">
+        <v>45943</v>
+      </c>
+      <c r="E572" s="11">
+        <v>59.9</v>
+      </c>
+      <c r="F572" s="11">
+        <v>0</v>
+      </c>
+      <c r="G572" s="11">
+        <v>0</v>
+      </c>
+      <c r="H572" s="11">
+        <v>9.4</v>
+      </c>
+      <c r="I572" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="573" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A573" s="7">
+        <v>3</v>
+      </c>
+      <c r="B573" s="7">
+        <v>572</v>
+      </c>
+      <c r="C573" s="8">
+        <v>45944</v>
+      </c>
+      <c r="E573" s="11">
+        <v>50.5</v>
+      </c>
+      <c r="F573" s="11">
+        <v>0</v>
+      </c>
+      <c r="G573" s="11">
+        <v>0</v>
+      </c>
+      <c r="H573" s="11">
+        <v>4</v>
+      </c>
+      <c r="I573" s="38"/>
+    </row>
+    <row r="574" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A574" s="7">
+        <v>4</v>
+      </c>
+      <c r="B574" s="7">
+        <v>573</v>
+      </c>
+      <c r="C574" s="8">
+        <v>45945</v>
+      </c>
+      <c r="E574" s="11">
+        <v>53</v>
+      </c>
+      <c r="F574" s="11">
+        <v>0.21</v>
+      </c>
+      <c r="G574" s="11">
+        <v>0</v>
+      </c>
+      <c r="H574" s="11">
+        <v>9</v>
+      </c>
+      <c r="I574" s="38"/>
+    </row>
+    <row r="575" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A575" s="7">
+        <v>5</v>
+      </c>
+      <c r="B575" s="7">
+        <v>574</v>
+      </c>
+      <c r="C575" s="8">
+        <v>45946</v>
+      </c>
+      <c r="E575" s="11">
+        <v>51.5</v>
+      </c>
+      <c r="F575" s="11">
+        <v>0</v>
+      </c>
+      <c r="G575" s="11">
+        <v>0</v>
+      </c>
+      <c r="H575" s="11">
+        <v>7</v>
+      </c>
+      <c r="I575" s="38"/>
+    </row>
+    <row r="576" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A576" s="7">
+        <v>6</v>
+      </c>
+      <c r="B576" s="7">
+        <v>575</v>
+      </c>
+      <c r="C576" s="8">
+        <v>45947</v>
+      </c>
+      <c r="E576" s="11">
+        <v>52</v>
+      </c>
+      <c r="F576" s="11">
+        <v>0</v>
+      </c>
+      <c r="G576" s="11">
+        <v>0</v>
+      </c>
+      <c r="H576" s="11">
+        <v>4</v>
+      </c>
+      <c r="I576" s="38"/>
+    </row>
+    <row r="577" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A577" s="7">
+        <v>7</v>
+      </c>
+      <c r="B577" s="7">
+        <v>576</v>
+      </c>
+      <c r="C577" s="8">
+        <v>45948</v>
+      </c>
+      <c r="E577" s="11">
+        <v>51.5</v>
+      </c>
+      <c r="F577" s="11">
+        <v>0</v>
+      </c>
+      <c r="G577" s="11">
+        <v>0</v>
+      </c>
+      <c r="H577" s="11">
+        <v>7</v>
+      </c>
+      <c r="I577" s="38"/>
+    </row>
+    <row r="578" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A578" s="7">
+        <v>1</v>
+      </c>
+      <c r="B578" s="7">
+        <v>577</v>
+      </c>
+      <c r="C578" s="8">
+        <v>45949</v>
+      </c>
+      <c r="E578" s="11">
+        <v>53.5</v>
+      </c>
+      <c r="F578" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="G578" s="11">
+        <v>0</v>
+      </c>
+      <c r="H578" s="11">
+        <v>8</v>
+      </c>
+      <c r="I578" s="38"/>
+    </row>
+    <row r="579" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A579" s="7">
+        <v>2</v>
+      </c>
+      <c r="B579" s="7">
+        <v>578</v>
+      </c>
+      <c r="C579" s="8">
+        <v>45950</v>
+      </c>
+      <c r="E579" s="11">
+        <v>55.5</v>
+      </c>
+      <c r="F579" s="11">
+        <v>0</v>
+      </c>
+      <c r="G579" s="11">
+        <v>0</v>
+      </c>
+      <c r="H579" s="11">
+        <v>14</v>
+      </c>
+      <c r="I579" s="38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A580" s="7">
+        <v>3</v>
+      </c>
+      <c r="B580" s="7">
+        <v>579</v>
+      </c>
+      <c r="C580" s="8">
+        <v>45951</v>
+      </c>
+      <c r="E580" s="11">
+        <v>55</v>
+      </c>
+      <c r="F580" s="11">
+        <v>0</v>
+      </c>
+      <c r="G580" s="11">
+        <v>0</v>
+      </c>
+      <c r="H580" s="11">
+        <v>14</v>
+      </c>
+      <c r="I580" s="38"/>
+    </row>
+    <row r="581" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A581" s="7">
+        <v>4</v>
+      </c>
+      <c r="B581" s="7">
+        <v>580</v>
+      </c>
+      <c r="C581" s="8">
+        <v>45952</v>
+      </c>
+      <c r="E581" s="11">
+        <v>54</v>
+      </c>
+      <c r="F581" s="11">
+        <v>0</v>
+      </c>
+      <c r="G581" s="11">
+        <v>0</v>
+      </c>
+      <c r="H581" s="11">
+        <v>6</v>
+      </c>
+      <c r="I581" s="38"/>
+    </row>
+    <row r="582" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A582" s="7">
+        <v>5</v>
+      </c>
+      <c r="B582" s="7">
+        <v>581</v>
+      </c>
+      <c r="C582" s="8">
+        <v>45953</v>
+      </c>
+      <c r="E582" s="11">
+        <v>54.5</v>
+      </c>
+      <c r="F582" s="11">
+        <v>0</v>
+      </c>
+      <c r="G582" s="11">
+        <v>0</v>
+      </c>
+      <c r="H582" s="11">
+        <v>5</v>
+      </c>
+      <c r="I582" s="38"/>
+    </row>
+    <row r="583" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A583" s="7">
+        <v>6</v>
+      </c>
+      <c r="B583" s="7">
+        <v>582</v>
+      </c>
+      <c r="C583" s="8">
+        <v>45954</v>
+      </c>
+      <c r="E583" s="11">
+        <v>55</v>
+      </c>
+      <c r="F583" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="G583" s="11">
+        <v>0</v>
+      </c>
+      <c r="H583" s="11">
+        <v>8</v>
+      </c>
+      <c r="I583" s="38"/>
+    </row>
+    <row r="584" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A584" s="7">
+        <v>7</v>
+      </c>
+      <c r="B584" s="7">
+        <v>583</v>
+      </c>
+      <c r="C584" s="8">
+        <v>45955</v>
+      </c>
+      <c r="E584" s="11">
+        <v>56</v>
+      </c>
+      <c r="F584" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G584" s="11">
+        <v>0</v>
+      </c>
+      <c r="H584" s="11">
+        <v>14</v>
+      </c>
+      <c r="I584" s="38"/>
+    </row>
+    <row r="585" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A585" s="7">
+        <v>1</v>
+      </c>
+      <c r="B585" s="7">
+        <v>584</v>
+      </c>
+      <c r="C585" s="8">
+        <v>45956</v>
+      </c>
+      <c r="E585" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="F585" s="11">
+        <v>0.61</v>
+      </c>
+      <c r="G585" s="11">
+        <v>0</v>
+      </c>
+      <c r="H585" s="11">
+        <v>15</v>
+      </c>
+      <c r="I585" s="38"/>
+    </row>
+    <row r="586" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A586" s="7">
+        <v>2</v>
+      </c>
+      <c r="B586" s="7">
+        <v>585</v>
+      </c>
+      <c r="C586" s="8">
+        <v>45957</v>
+      </c>
+      <c r="E586" s="11">
+        <v>51.5</v>
+      </c>
+      <c r="F586" s="11">
+        <v>0</v>
+      </c>
+      <c r="G586" s="11">
+        <v>0</v>
+      </c>
+      <c r="H586" s="11">
+        <v>8</v>
+      </c>
+      <c r="I586" s="38"/>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A587" s="7">
+        <v>3</v>
+      </c>
+      <c r="B587" s="7">
+        <v>586</v>
+      </c>
+      <c r="C587" s="8">
+        <v>45958</v>
+      </c>
+      <c r="E587" s="11">
+        <v>49</v>
+      </c>
+      <c r="F587" s="11">
+        <v>0</v>
+      </c>
+      <c r="G587" s="11">
+        <v>0</v>
+      </c>
+      <c r="H587" s="11">
+        <v>7</v>
+      </c>
+      <c r="I587" s="38"/>
+    </row>
+    <row r="588" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A588" s="7">
+        <v>4</v>
+      </c>
+      <c r="B588" s="7">
+        <v>587</v>
+      </c>
+      <c r="C588" s="8">
+        <v>45959</v>
+      </c>
+      <c r="E588" s="11">
+        <v>52.5</v>
+      </c>
+      <c r="F588" s="11">
+        <v>0</v>
+      </c>
+      <c r="G588" s="11">
+        <v>0</v>
+      </c>
+      <c r="H588" s="11">
+        <v>12</v>
+      </c>
+      <c r="I588" s="38"/>
+    </row>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A589" s="7">
+        <v>5</v>
+      </c>
+      <c r="B589" s="7">
+        <v>588</v>
+      </c>
+      <c r="C589" s="8">
+        <v>45960</v>
+      </c>
+      <c r="E589" s="11">
+        <v>51.5</v>
+      </c>
+      <c r="F589" s="11">
+        <v>0</v>
+      </c>
+      <c r="G589" s="11">
+        <v>0</v>
+      </c>
+      <c r="H589" s="11">
+        <v>5</v>
+      </c>
+      <c r="I589" s="38"/>
+    </row>
+    <row r="590" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A590" s="7">
+        <v>6</v>
+      </c>
+      <c r="B590" s="7">
+        <v>589</v>
+      </c>
+      <c r="C590" s="8">
+        <v>45961</v>
+      </c>
+      <c r="E590" s="11">
+        <v>50</v>
+      </c>
+      <c r="F590" s="11">
+        <v>0</v>
+      </c>
+      <c r="G590" s="11">
+        <v>0</v>
+      </c>
+      <c r="H590" s="11">
+        <v>7</v>
+      </c>
+      <c r="I590" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="591" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A591" s="7">
+        <v>7</v>
+      </c>
+      <c r="B591" s="7">
+        <v>590</v>
+      </c>
+      <c r="C591" s="8">
+        <v>45962</v>
+      </c>
+      <c r="E591" s="11">
+        <v>52</v>
+      </c>
+      <c r="F591" s="11">
+        <v>0</v>
+      </c>
+      <c r="G591" s="11">
+        <v>0</v>
+      </c>
+      <c r="H591" s="11">
+        <v>9</v>
+      </c>
+      <c r="I591" s="38"/>
+    </row>
+    <row r="592" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A592" s="7">
+        <v>1</v>
+      </c>
+      <c r="B592" s="7">
+        <v>591</v>
+      </c>
+      <c r="C592" s="8">
+        <v>45963</v>
+      </c>
+      <c r="E592" s="11">
+        <v>51</v>
+      </c>
+      <c r="F592" s="11">
+        <v>0</v>
+      </c>
+      <c r="G592" s="11">
+        <v>0</v>
+      </c>
+      <c r="H592" s="11">
+        <v>10</v>
+      </c>
+      <c r="I592" s="38"/>
+    </row>
+    <row r="593" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A593" s="7">
+        <v>2</v>
+      </c>
+      <c r="B593" s="7">
+        <v>592</v>
+      </c>
+      <c r="C593" s="8">
+        <v>45964</v>
+      </c>
+      <c r="E593" s="11">
+        <v>48.5</v>
+      </c>
+      <c r="F593" s="11">
+        <v>0</v>
+      </c>
+      <c r="G593" s="11">
+        <v>0</v>
+      </c>
+      <c r="H593" s="11">
+        <v>4</v>
+      </c>
+      <c r="I593" s="38"/>
+    </row>
+    <row r="594" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A594" s="7">
+        <v>3</v>
+      </c>
+      <c r="B594" s="7">
+        <v>593</v>
+      </c>
+      <c r="C594" s="8">
+        <v>45965</v>
+      </c>
+      <c r="E594" s="11">
+        <v>50.5</v>
+      </c>
+      <c r="F594" s="11">
+        <v>0</v>
+      </c>
+      <c r="G594" s="11">
+        <v>0</v>
+      </c>
+      <c r="H594" s="11">
+        <v>10</v>
+      </c>
+      <c r="I594" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A595" s="7">
+        <v>4</v>
+      </c>
+      <c r="B595" s="7">
+        <v>594</v>
+      </c>
+      <c r="C595" s="8">
+        <v>45966</v>
+      </c>
+      <c r="E595" s="11">
+        <v>50.5</v>
+      </c>
+      <c r="F595" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G595" s="11">
+        <v>0</v>
+      </c>
+      <c r="H595" s="11">
+        <v>7</v>
+      </c>
+      <c r="I595" s="38"/>
+    </row>
+    <row r="596" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A596" s="7">
+        <v>5</v>
+      </c>
+      <c r="B596" s="7">
+        <v>595</v>
+      </c>
+      <c r="C596" s="8">
+        <v>45967</v>
+      </c>
+      <c r="E596" s="11">
+        <v>49.5</v>
+      </c>
+      <c r="F596" s="11">
+        <v>0</v>
+      </c>
+      <c r="G596" s="11">
+        <v>0</v>
+      </c>
+      <c r="H596" s="11">
+        <v>6</v>
+      </c>
+      <c r="I596" s="38"/>
+    </row>
+    <row r="597" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A597" s="7">
+        <v>6</v>
+      </c>
+      <c r="B597" s="7">
+        <v>596</v>
+      </c>
+      <c r="C597" s="8">
+        <v>45968</v>
+      </c>
+      <c r="E597" s="11">
+        <v>43.5</v>
+      </c>
+      <c r="F597" s="11">
+        <v>0</v>
+      </c>
+      <c r="G597" s="11">
+        <v>0</v>
+      </c>
+      <c r="H597" s="11">
+        <v>13</v>
+      </c>
+      <c r="I597" s="38"/>
+    </row>
+    <row r="598" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A598" s="7">
+        <v>7</v>
+      </c>
+      <c r="B598" s="7">
+        <v>597</v>
+      </c>
+      <c r="C598" s="8">
+        <v>45969</v>
+      </c>
+      <c r="E598" s="11">
+        <v>39</v>
+      </c>
+      <c r="F598" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="G598" s="11">
         <v>0.1</v>
       </c>
-      <c r="G548" s="11">
-        <v>0</v>
-      </c>
-      <c r="H548" s="11">
+      <c r="H598" s="11">
+        <v>8</v>
+      </c>
+      <c r="I598" s="38"/>
+    </row>
+    <row r="599" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A599" s="7">
+        <v>1</v>
+      </c>
+      <c r="B599" s="7">
+        <v>598</v>
+      </c>
+      <c r="C599" s="8">
+        <v>45970</v>
+      </c>
+      <c r="E599" s="11">
+        <v>43</v>
+      </c>
+      <c r="F599" s="11">
+        <v>0.04</v>
+      </c>
+      <c r="G599" s="11">
+        <v>0</v>
+      </c>
+      <c r="H599" s="11">
         <v>9</v>
       </c>
-      <c r="J548" s="37">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="549" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A549" s="7"/>
-      <c r="B549" s="7"/>
-      <c r="C549" s="8"/>
-    </row>
-    <row r="550" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A550" s="7"/>
-    </row>
-    <row r="551" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A551" s="7"/>
-    </row>
-    <row r="552" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A552" s="7"/>
-    </row>
-    <row r="553" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A553" s="7"/>
+      <c r="I599" s="38"/>
+    </row>
+    <row r="600" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A600" s="7">
+        <v>2</v>
+      </c>
+      <c r="B600" s="7">
+        <v>599</v>
+      </c>
+      <c r="C600" s="8">
+        <v>45971</v>
+      </c>
+      <c r="E600" s="11">
+        <v>46.5</v>
+      </c>
+      <c r="F600" s="11">
+        <v>0</v>
+      </c>
+      <c r="G600" s="11">
+        <v>0</v>
+      </c>
+      <c r="H600" s="11">
+        <v>6</v>
+      </c>
+      <c r="I600" s="38"/>
+    </row>
+    <row r="601" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A601" s="7">
+        <v>3</v>
+      </c>
+      <c r="B601" s="7">
+        <v>600</v>
+      </c>
+      <c r="C601" s="8">
+        <v>45972</v>
+      </c>
+      <c r="E601" s="11">
+        <v>42.5</v>
+      </c>
+      <c r="F601" s="11">
+        <v>0</v>
+      </c>
+      <c r="G601" s="11">
+        <v>0</v>
+      </c>
+      <c r="H601" s="11">
+        <v>10</v>
+      </c>
+      <c r="I601" s="38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="602" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A602" s="7">
+        <v>4</v>
+      </c>
+      <c r="B602" s="7">
+        <v>601</v>
+      </c>
+      <c r="C602" s="8">
+        <v>45973</v>
+      </c>
+      <c r="E602" s="11">
+        <v>39.5</v>
+      </c>
+      <c r="F602" s="11">
+        <v>0</v>
+      </c>
+      <c r="G602" s="11">
+        <v>0</v>
+      </c>
+      <c r="H602" s="11">
+        <v>12</v>
+      </c>
+      <c r="I602" s="38"/>
+    </row>
+    <row r="603" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A603" s="7">
+        <v>5</v>
+      </c>
+      <c r="B603" s="7">
+        <v>602</v>
+      </c>
+      <c r="C603" s="8">
+        <v>45974</v>
+      </c>
+      <c r="E603" s="11">
+        <v>34.5</v>
+      </c>
+      <c r="F603" s="11">
+        <v>0</v>
+      </c>
+      <c r="G603" s="11">
+        <v>0</v>
+      </c>
+      <c r="H603" s="11">
+        <v>9</v>
+      </c>
+      <c r="I603" s="38"/>
+    </row>
+    <row r="604" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A604" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15452,20 +16813,20 @@
         <v>43</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="38">
+      <c r="C1" s="39">
         <v>0.85</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="41"/>
       <c r="O1" s="24" t="s">
         <v>39</v>
       </c>
@@ -19032,7 +20393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2573A6AB-8DBE-4210-8EFE-4E449AA3F45B}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H65" sqref="H65:H72"/>
     </sheetView>
   </sheetViews>
@@ -19046,20 +20407,20 @@
         <v>43</v>
       </c>
       <c r="B1" s="8"/>
-      <c r="C1" s="38">
+      <c r="C1" s="39">
         <v>0.85</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="41"/>
       <c r="O1" s="24" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
tweeked the sliding windows to try and be more accurate to conditions
</commit_message>
<xml_diff>
--- a/restaurant_analytics/data/mornings.xlsx
+++ b/restaurant_analytics/data/mornings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cardi\Documents\git-repo\swe_dev\restaurant_analytics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E46ADF3-3446-4443-8C8D-D209C46ED8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393A0407-58DF-4887-91F9-4C54AD79C635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32025" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>day</t>
   </si>
@@ -216,25 +216,13 @@
   <si>
     <t>trn %</t>
   </si>
-  <si>
-    <t>avg1</t>
-  </si>
-  <si>
-    <t>std1</t>
-  </si>
-  <si>
-    <t>avg2</t>
-  </si>
-  <si>
-    <t>std2</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -579,6 +567,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,8 +587,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,14 +615,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -983,11 +971,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O722"/>
+  <dimension ref="A1:K722"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A644" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J665" sqref="J665"/>
+      <pane ySplit="1" topLeftCell="A668" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B685" sqref="B685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18332,7 +18320,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="657" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A657" s="6">
         <v>3</v>
       </c>
@@ -18358,7 +18346,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="658" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A658" s="6">
         <v>4</v>
       </c>
@@ -18384,7 +18372,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="659" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A659" s="6">
         <v>5</v>
       </c>
@@ -18410,7 +18398,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="660" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A660" s="6">
         <v>6</v>
       </c>
@@ -18436,7 +18424,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="661" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A661" s="6">
         <v>7</v>
       </c>
@@ -18461,20 +18449,8 @@
       <c r="H661" s="9">
         <v>10.6</v>
       </c>
-      <c r="L661" t="s">
-        <v>59</v>
-      </c>
-      <c r="M661" t="s">
-        <v>60</v>
-      </c>
-      <c r="N661" t="s">
-        <v>61</v>
-      </c>
-      <c r="O661" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="662" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="662" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A662" s="6">
         <v>1</v>
       </c>
@@ -18499,20 +18475,8 @@
       <c r="H662" s="9">
         <v>12.7</v>
       </c>
-      <c r="L662">
-        <v>29</v>
-      </c>
-      <c r="M662">
-        <v>9.7200000000000006</v>
-      </c>
-      <c r="N662">
-        <v>20</v>
-      </c>
-      <c r="O662">
-        <v>8.76</v>
-      </c>
-    </row>
-    <row r="663" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="663" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A663" s="6">
         <v>2</v>
       </c>
@@ -18522,6 +18486,9 @@
       <c r="C663" s="7">
         <v>46034</v>
       </c>
+      <c r="D663" s="14">
+        <v>7</v>
+      </c>
       <c r="E663" s="9">
         <v>34.299999999999997</v>
       </c>
@@ -18534,20 +18501,8 @@
       <c r="H663" s="9">
         <v>12.5</v>
       </c>
-      <c r="L663">
-        <v>20</v>
-      </c>
-      <c r="M663">
-        <v>6.82</v>
-      </c>
-      <c r="N663">
-        <v>13</v>
-      </c>
-      <c r="O663">
-        <v>6.05</v>
-      </c>
-    </row>
-    <row r="664" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="664" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A664" s="6">
         <v>3</v>
       </c>
@@ -18557,6 +18512,9 @@
       <c r="C664" s="7">
         <v>46035</v>
       </c>
+      <c r="D664" s="14">
+        <v>2</v>
+      </c>
       <c r="E664" s="9">
         <v>39.9</v>
       </c>
@@ -18569,20 +18527,8 @@
       <c r="H664" s="9">
         <v>15</v>
       </c>
-      <c r="L664">
-        <v>26</v>
-      </c>
-      <c r="M664">
-        <v>6.73</v>
-      </c>
-      <c r="N664">
-        <v>20</v>
-      </c>
-      <c r="O664">
-        <v>9.24</v>
-      </c>
-    </row>
-    <row r="665" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="665" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A665" s="6">
         <v>4</v>
       </c>
@@ -18592,6 +18538,9 @@
       <c r="C665" s="7">
         <v>46036</v>
       </c>
+      <c r="D665" s="14">
+        <v>21</v>
+      </c>
       <c r="E665" s="9">
         <v>29.5</v>
       </c>
@@ -18604,20 +18553,8 @@
       <c r="H665" s="9">
         <v>17</v>
       </c>
-      <c r="L665">
-        <v>16</v>
-      </c>
-      <c r="M665">
-        <v>6.17</v>
-      </c>
-      <c r="N665">
-        <v>12</v>
-      </c>
-      <c r="O665">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
-    <row r="666" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="666" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A666" s="6">
         <v>5</v>
       </c>
@@ -18627,6 +18564,9 @@
       <c r="C666" s="7">
         <v>46037</v>
       </c>
+      <c r="D666" s="14">
+        <v>11</v>
+      </c>
       <c r="E666" s="9">
         <v>21.9</v>
       </c>
@@ -18639,20 +18579,8 @@
       <c r="H666" s="9">
         <v>10</v>
       </c>
-      <c r="L666">
-        <v>9</v>
-      </c>
-      <c r="M666">
-        <v>4.99</v>
-      </c>
-      <c r="N666">
-        <v>7</v>
-      </c>
-      <c r="O666">
-        <v>2.41</v>
-      </c>
-    </row>
-    <row r="667" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="667" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A667" s="6">
         <v>6</v>
       </c>
@@ -18662,6 +18590,9 @@
       <c r="C667" s="7">
         <v>46038</v>
       </c>
+      <c r="D667" s="14">
+        <v>0</v>
+      </c>
       <c r="E667" s="9">
         <v>25.2</v>
       </c>
@@ -18674,20 +18605,8 @@
       <c r="H667" s="9">
         <v>10.1</v>
       </c>
-      <c r="L667">
-        <v>29</v>
-      </c>
-      <c r="M667">
-        <v>12.42</v>
-      </c>
-      <c r="N667">
-        <v>25</v>
-      </c>
-      <c r="O667">
-        <v>13.75</v>
-      </c>
-    </row>
-    <row r="668" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="668" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A668" s="6">
         <v>7</v>
       </c>
@@ -18697,6 +18616,9 @@
       <c r="C668" s="7">
         <v>46039</v>
       </c>
+      <c r="D668" s="14">
+        <v>15</v>
+      </c>
       <c r="E668" s="9">
         <v>20.5</v>
       </c>
@@ -18709,20 +18631,8 @@
       <c r="H668" s="9">
         <v>11.2</v>
       </c>
-      <c r="L668">
-        <v>13</v>
-      </c>
-      <c r="M668">
-        <v>4.6900000000000004</v>
-      </c>
-      <c r="N668">
-        <v>10</v>
-      </c>
-      <c r="O668">
-        <v>4.88</v>
-      </c>
-    </row>
-    <row r="669" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="669" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A669" s="6">
         <v>1</v>
       </c>
@@ -18732,6 +18642,9 @@
       <c r="C669" s="7">
         <v>46040</v>
       </c>
+      <c r="D669" s="14">
+        <v>25</v>
+      </c>
       <c r="E669" s="9">
         <v>16.5</v>
       </c>
@@ -18744,20 +18657,8 @@
       <c r="H669" s="9">
         <v>11.5</v>
       </c>
-      <c r="L669">
-        <v>30</v>
-      </c>
-      <c r="M669">
-        <v>10.25</v>
-      </c>
-      <c r="N669">
-        <v>20</v>
-      </c>
-      <c r="O669">
-        <v>6.58</v>
-      </c>
-    </row>
-    <row r="670" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="670" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A670" s="6">
         <v>2</v>
       </c>
@@ -18767,6 +18668,9 @@
       <c r="C670" s="7">
         <v>46041</v>
       </c>
+      <c r="D670" s="14">
+        <v>21</v>
+      </c>
       <c r="E670" s="9">
         <v>14.5</v>
       </c>
@@ -18782,20 +18686,8 @@
       <c r="I670" t="s">
         <v>32</v>
       </c>
-      <c r="L670">
-        <v>11</v>
-      </c>
-      <c r="M670">
-        <v>9.69</v>
-      </c>
-      <c r="N670">
-        <v>6</v>
-      </c>
-      <c r="O670">
-        <v>3.22</v>
-      </c>
-    </row>
-    <row r="671" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="671" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A671" s="6">
         <v>3</v>
       </c>
@@ -18805,6 +18697,9 @@
       <c r="C671" s="7">
         <v>46042</v>
       </c>
+      <c r="D671" s="14">
+        <v>5</v>
+      </c>
       <c r="E671" s="9">
         <v>16.7</v>
       </c>
@@ -18817,20 +18712,8 @@
       <c r="H671" s="9">
         <v>10.4</v>
       </c>
-      <c r="L671">
-        <v>13</v>
-      </c>
-      <c r="M671">
-        <v>9.01</v>
-      </c>
-      <c r="N671">
-        <v>8</v>
-      </c>
-      <c r="O671">
-        <v>4.6399999999999997</v>
-      </c>
-    </row>
-    <row r="672" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="672" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A672" s="6">
         <v>4</v>
       </c>
@@ -18840,6 +18723,9 @@
       <c r="C672" s="7">
         <v>46043</v>
       </c>
+      <c r="D672" s="14">
+        <v>18</v>
+      </c>
       <c r="E672" s="9">
         <v>30.5</v>
       </c>
@@ -18852,20 +18738,8 @@
       <c r="H672" s="9">
         <v>12</v>
       </c>
-      <c r="L672">
-        <v>17</v>
-      </c>
-      <c r="M672">
-        <v>5.9</v>
-      </c>
-      <c r="N672">
-        <v>13</v>
-      </c>
-      <c r="O672">
-        <v>5.37</v>
-      </c>
-    </row>
-    <row r="673" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="673" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A673" s="6">
         <v>5</v>
       </c>
@@ -18875,6 +18749,9 @@
       <c r="C673" s="7">
         <v>46044</v>
       </c>
+      <c r="D673" s="14">
+        <v>12</v>
+      </c>
       <c r="E673" s="9">
         <v>26.5</v>
       </c>
@@ -18887,20 +18764,8 @@
       <c r="H673" s="9">
         <v>9</v>
       </c>
-      <c r="L673">
-        <v>19</v>
-      </c>
-      <c r="M673">
-        <v>5.37</v>
-      </c>
-      <c r="N673">
-        <v>15</v>
-      </c>
-      <c r="O673">
-        <v>5.36</v>
-      </c>
-    </row>
-    <row r="674" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="674" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A674" s="6">
         <v>6</v>
       </c>
@@ -18910,6 +18775,9 @@
       <c r="C674" s="7">
         <v>46045</v>
       </c>
+      <c r="D674" s="14">
+        <v>7</v>
+      </c>
       <c r="E674" s="9">
         <v>24</v>
       </c>
@@ -18922,20 +18790,8 @@
       <c r="H674" s="9">
         <v>13</v>
       </c>
-      <c r="L674">
-        <v>13</v>
-      </c>
-      <c r="M674">
-        <v>5.14</v>
-      </c>
-      <c r="N674">
-        <v>11</v>
-      </c>
-      <c r="O674">
-        <v>5.36</v>
-      </c>
-    </row>
-    <row r="675" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="675" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A675" s="6">
         <v>7</v>
       </c>
@@ -18945,6 +18801,9 @@
       <c r="C675" s="7">
         <v>46046</v>
       </c>
+      <c r="D675" s="14">
+        <v>26</v>
+      </c>
       <c r="E675" s="9">
         <v>22</v>
       </c>
@@ -18957,20 +18816,8 @@
       <c r="H675" s="9">
         <v>12</v>
       </c>
-      <c r="L675">
-        <v>19</v>
-      </c>
-      <c r="M675">
-        <v>7.81</v>
-      </c>
-      <c r="N675">
-        <v>16</v>
-      </c>
-      <c r="O675">
-        <v>8.8699999999999992</v>
-      </c>
-    </row>
-    <row r="676" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="676" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A676" s="6">
         <v>1</v>
       </c>
@@ -18980,6 +18827,9 @@
       <c r="C676" s="7">
         <v>46047</v>
       </c>
+      <c r="D676" s="14">
+        <v>36</v>
+      </c>
       <c r="E676" s="9">
         <v>15</v>
       </c>
@@ -18992,20 +18842,8 @@
       <c r="H676" s="9">
         <v>4</v>
       </c>
-      <c r="L676">
-        <v>39</v>
-      </c>
-      <c r="M676">
-        <v>14.02</v>
-      </c>
-      <c r="N676">
-        <v>29</v>
-      </c>
-      <c r="O676">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="677" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="677" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A677" s="6">
         <v>2</v>
       </c>
@@ -19015,6 +18853,9 @@
       <c r="C677" s="7">
         <v>46048</v>
       </c>
+      <c r="D677" s="14">
+        <v>11</v>
+      </c>
       <c r="E677" s="9">
         <v>15</v>
       </c>
@@ -19027,20 +18868,8 @@
       <c r="H677" s="9">
         <v>5</v>
       </c>
-      <c r="L677">
-        <v>25</v>
-      </c>
-      <c r="M677">
-        <v>12.02</v>
-      </c>
-      <c r="N677">
-        <v>16</v>
-      </c>
-      <c r="O677">
-        <v>6.87</v>
-      </c>
-    </row>
-    <row r="678" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="678" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A678" s="6">
         <v>3</v>
       </c>
@@ -19050,6 +18879,9 @@
       <c r="C678" s="7">
         <v>46049</v>
       </c>
+      <c r="D678" s="14">
+        <v>9</v>
+      </c>
       <c r="E678" s="9">
         <v>15</v>
       </c>
@@ -19062,20 +18894,8 @@
       <c r="H678" s="9">
         <v>6</v>
       </c>
-      <c r="L678">
-        <v>11</v>
-      </c>
-      <c r="M678">
-        <v>10.19</v>
-      </c>
-      <c r="N678">
-        <v>6</v>
-      </c>
-      <c r="O678">
-        <v>3.77</v>
-      </c>
-    </row>
-    <row r="679" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="679" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A679" s="6">
         <v>4</v>
       </c>
@@ -19085,6 +18905,9 @@
       <c r="C679" s="7">
         <v>46050</v>
       </c>
+      <c r="D679" s="14">
+        <v>14</v>
+      </c>
       <c r="E679" s="9">
         <v>25</v>
       </c>
@@ -19097,20 +18920,8 @@
       <c r="H679" s="9">
         <v>13</v>
       </c>
-      <c r="L679">
-        <v>15</v>
-      </c>
-      <c r="M679">
-        <v>5.7</v>
-      </c>
-      <c r="N679">
-        <v>11</v>
-      </c>
-      <c r="O679">
-        <v>4.3899999999999997</v>
-      </c>
-    </row>
-    <row r="680" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="680" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A680" s="6">
         <v>5</v>
       </c>
@@ -19120,6 +18931,9 @@
       <c r="C680" s="7">
         <v>46051</v>
       </c>
+      <c r="D680" s="14">
+        <v>10</v>
+      </c>
       <c r="E680" s="9">
         <v>31</v>
       </c>
@@ -19132,20 +18946,8 @@
       <c r="H680" s="9">
         <v>9</v>
       </c>
-      <c r="L680">
-        <v>14</v>
-      </c>
-      <c r="M680">
-        <v>5.25</v>
-      </c>
-      <c r="N680">
-        <v>12</v>
-      </c>
-      <c r="O680">
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="681" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="681" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A681" s="6">
         <v>6</v>
       </c>
@@ -19155,6 +18957,9 @@
       <c r="C681" s="7">
         <v>46052</v>
       </c>
+      <c r="D681" s="14">
+        <v>19</v>
+      </c>
       <c r="E681" s="9">
         <v>24</v>
       </c>
@@ -19167,20 +18972,8 @@
       <c r="H681" s="9">
         <v>17</v>
       </c>
-      <c r="L681">
-        <v>22</v>
-      </c>
-      <c r="M681">
-        <v>9.6300000000000008</v>
-      </c>
-      <c r="N681">
-        <v>18</v>
-      </c>
-      <c r="O681">
-        <v>11.08</v>
-      </c>
-    </row>
-    <row r="682" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="682" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A682" s="6">
         <v>7</v>
       </c>
@@ -19190,6 +18983,9 @@
       <c r="C682" s="7">
         <v>46053</v>
       </c>
+      <c r="D682" s="14">
+        <v>28</v>
+      </c>
       <c r="E682" s="9">
         <v>14.5</v>
       </c>
@@ -19202,20 +18998,8 @@
       <c r="H682" s="9">
         <v>9</v>
       </c>
-      <c r="L682">
-        <v>18</v>
-      </c>
-      <c r="M682">
-        <v>5.73</v>
-      </c>
-      <c r="N682">
-        <v>15</v>
-      </c>
-      <c r="O682">
-        <v>7.18</v>
-      </c>
-    </row>
-    <row r="683" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="683" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A683" s="6">
         <v>1</v>
       </c>
@@ -19225,6 +19009,9 @@
       <c r="C683" s="7">
         <v>46054</v>
       </c>
+      <c r="D683" s="14">
+        <v>11</v>
+      </c>
       <c r="E683" s="9">
         <v>22.5</v>
       </c>
@@ -19237,20 +19024,8 @@
       <c r="H683" s="9">
         <v>13</v>
       </c>
-      <c r="L683">
-        <v>27</v>
-      </c>
-      <c r="M683">
-        <v>9.32</v>
-      </c>
-      <c r="N683">
-        <v>19</v>
-      </c>
-      <c r="O683">
-        <v>7.73</v>
-      </c>
-    </row>
-    <row r="684" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="684" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A684" s="6">
         <v>2</v>
       </c>
@@ -19260,6 +19035,9 @@
       <c r="C684" s="7">
         <v>46055</v>
       </c>
+      <c r="D684" s="14">
+        <v>4</v>
+      </c>
       <c r="E684" s="9">
         <v>23</v>
       </c>
@@ -19272,20 +19050,8 @@
       <c r="H684" s="9">
         <v>15</v>
       </c>
-      <c r="L684">
-        <v>11</v>
-      </c>
-      <c r="M684">
-        <v>6.52</v>
-      </c>
-      <c r="N684">
-        <v>6</v>
-      </c>
-      <c r="O684">
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="685" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="685" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A685" s="6">
         <v>3</v>
       </c>
@@ -19295,6 +19061,9 @@
       <c r="C685" s="7">
         <v>46056</v>
       </c>
+      <c r="D685" s="14">
+        <v>1</v>
+      </c>
       <c r="E685" s="9">
         <v>17</v>
       </c>
@@ -19307,20 +19076,8 @@
       <c r="H685" s="9">
         <v>5</v>
       </c>
-      <c r="L685">
-        <v>14</v>
-      </c>
-      <c r="M685">
-        <v>9.17</v>
-      </c>
-      <c r="N685">
-        <v>10</v>
-      </c>
-      <c r="O685">
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="686" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="686" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A686" s="6">
         <v>4</v>
       </c>
@@ -19330,6 +19087,9 @@
       <c r="C686" s="7">
         <v>46057</v>
       </c>
+      <c r="D686" s="14">
+        <v>11.5</v>
+      </c>
       <c r="E686" s="9">
         <v>18</v>
       </c>
@@ -19342,20 +19102,11 @@
       <c r="H686" s="9">
         <v>14</v>
       </c>
-      <c r="L686">
-        <v>13</v>
-      </c>
-      <c r="M686">
-        <v>5.55</v>
-      </c>
-      <c r="N686">
-        <v>10</v>
-      </c>
-      <c r="O686">
-        <v>4.53</v>
-      </c>
-    </row>
-    <row r="687" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J686" s="9">
+        <v>5.04</v>
+      </c>
+    </row>
+    <row r="687" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A687" s="6">
         <v>5</v>
       </c>
@@ -19365,6 +19116,9 @@
       <c r="C687" s="7">
         <v>46058</v>
       </c>
+      <c r="D687" s="14">
+        <v>15</v>
+      </c>
       <c r="E687" s="9">
         <v>16</v>
       </c>
@@ -19377,20 +19131,11 @@
       <c r="H687" s="9">
         <v>8</v>
       </c>
-      <c r="L687">
-        <v>17</v>
-      </c>
-      <c r="M687">
-        <v>5.45</v>
-      </c>
-      <c r="N687">
-        <v>13</v>
-      </c>
-      <c r="O687">
-        <v>5.77</v>
-      </c>
-    </row>
-    <row r="688" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J687" s="9">
+        <v>5.6099999999999994</v>
+      </c>
+    </row>
+    <row r="688" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A688" s="6">
         <v>6</v>
       </c>
@@ -19400,6 +19145,9 @@
       <c r="C688" s="7">
         <v>46059</v>
       </c>
+      <c r="D688" s="14">
+        <v>18</v>
+      </c>
       <c r="E688" s="9">
         <v>18.5</v>
       </c>
@@ -19412,20 +19160,11 @@
       <c r="H688" s="9">
         <v>6</v>
       </c>
-      <c r="L688">
-        <v>19</v>
-      </c>
-      <c r="M688">
-        <v>6.69</v>
-      </c>
-      <c r="N688">
-        <v>17</v>
-      </c>
-      <c r="O688">
-        <v>5.55</v>
-      </c>
-    </row>
-    <row r="689" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J688" s="9">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="689" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A689" s="6">
         <v>7</v>
       </c>
@@ -19435,6 +19174,9 @@
       <c r="C689" s="7">
         <v>46060</v>
       </c>
+      <c r="D689" s="14">
+        <v>14</v>
+      </c>
       <c r="E689" s="9">
         <v>17</v>
       </c>
@@ -19447,20 +19189,11 @@
       <c r="H689" s="9">
         <v>10</v>
       </c>
-      <c r="L689">
-        <v>15</v>
-      </c>
-      <c r="M689">
-        <v>3.85</v>
-      </c>
-      <c r="N689">
-        <v>13</v>
-      </c>
-      <c r="O689">
-        <v>5.08</v>
-      </c>
-    </row>
-    <row r="690" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J689" s="9">
+        <v>4.4649999999999999</v>
+      </c>
+    </row>
+    <row r="690" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A690" s="6">
         <v>1</v>
       </c>
@@ -19470,6 +19203,9 @@
       <c r="C690" s="7">
         <v>46061</v>
       </c>
+      <c r="D690" s="14">
+        <v>11.5</v>
+      </c>
       <c r="E690" s="9">
         <v>15.5</v>
       </c>
@@ -19485,20 +19221,11 @@
       <c r="I690" t="s">
         <v>33</v>
       </c>
-      <c r="L690">
-        <v>13</v>
-      </c>
-      <c r="M690">
-        <v>13.45</v>
-      </c>
-      <c r="N690">
-        <v>10</v>
-      </c>
-      <c r="O690">
-        <v>10.45</v>
-      </c>
-    </row>
-    <row r="691" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J690" s="9">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="691" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A691" s="6">
         <v>2</v>
       </c>
@@ -19508,6 +19235,9 @@
       <c r="C691" s="7">
         <v>46062</v>
       </c>
+      <c r="D691" s="14">
+        <v>22.5</v>
+      </c>
       <c r="E691" s="9">
         <v>14.5</v>
       </c>
@@ -19520,20 +19250,11 @@
       <c r="H691" s="9">
         <v>16</v>
       </c>
-      <c r="L691">
-        <v>26</v>
-      </c>
-      <c r="M691">
-        <v>8.1</v>
-      </c>
-      <c r="N691">
-        <v>19</v>
-      </c>
-      <c r="O691">
-        <v>7.78</v>
-      </c>
-    </row>
-    <row r="692" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J691" s="9">
+        <v>7.9399999999999995</v>
+      </c>
+    </row>
+    <row r="692" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A692" s="6">
         <v>3</v>
       </c>
@@ -19543,6 +19264,9 @@
       <c r="C692" s="7">
         <v>46063</v>
       </c>
+      <c r="D692" s="14">
+        <v>6.5</v>
+      </c>
       <c r="E692" s="9">
         <v>16.5</v>
       </c>
@@ -19555,20 +19279,11 @@
       <c r="H692" s="9">
         <v>13</v>
       </c>
-      <c r="L692">
-        <v>8</v>
-      </c>
-      <c r="M692">
-        <v>6.87</v>
-      </c>
-      <c r="N692">
-        <v>5</v>
-      </c>
-      <c r="O692">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="693" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J692" s="9">
+        <v>4.9350000000000005</v>
+      </c>
+    </row>
+    <row r="693" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A693" s="6">
         <v>4</v>
       </c>
@@ -19578,6 +19293,9 @@
       <c r="C693" s="7">
         <v>46064</v>
       </c>
+      <c r="D693" s="14">
+        <v>9</v>
+      </c>
       <c r="E693" s="9">
         <v>16.5</v>
       </c>
@@ -19590,20 +19308,11 @@
       <c r="H693" s="9">
         <v>6</v>
       </c>
-      <c r="L693">
-        <v>10</v>
-      </c>
-      <c r="M693">
-        <v>6.5</v>
-      </c>
-      <c r="N693">
-        <v>8</v>
-      </c>
-      <c r="O693">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="694" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J693" s="9">
+        <v>4.8250000000000002</v>
+      </c>
+    </row>
+    <row r="694" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A694" s="6">
         <v>5</v>
       </c>
@@ -19613,6 +19322,9 @@
       <c r="C694" s="7">
         <v>46065</v>
       </c>
+      <c r="D694" s="14">
+        <v>11</v>
+      </c>
       <c r="E694" s="9">
         <v>17</v>
       </c>
@@ -19625,20 +19337,11 @@
       <c r="H694" s="9">
         <v>5</v>
       </c>
-      <c r="L694">
-        <v>11</v>
-      </c>
-      <c r="M694">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="N694">
-        <v>11</v>
-      </c>
-      <c r="O694">
-        <v>2.82</v>
-      </c>
-    </row>
-    <row r="695" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J694" s="9">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="695" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A695" s="6">
         <v>6</v>
       </c>
@@ -19648,6 +19351,9 @@
       <c r="C695" s="7">
         <v>46066</v>
       </c>
+      <c r="D695" s="14">
+        <v>12.5</v>
+      </c>
       <c r="E695" s="9">
         <v>17</v>
       </c>
@@ -19660,20 +19366,11 @@
       <c r="H695" s="9">
         <v>6</v>
       </c>
-      <c r="L695">
-        <v>13</v>
-      </c>
-      <c r="M695">
-        <v>4.46</v>
-      </c>
-      <c r="N695">
-        <v>12</v>
-      </c>
-      <c r="O695">
-        <v>3.34</v>
-      </c>
-    </row>
-    <row r="696" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J695" s="9">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="696" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A696" s="6">
         <v>7</v>
       </c>
@@ -19683,6 +19380,9 @@
       <c r="C696" s="7">
         <v>46067</v>
       </c>
+      <c r="D696" s="14">
+        <v>18.5</v>
+      </c>
       <c r="E696" s="9">
         <v>17</v>
       </c>
@@ -19698,20 +19398,11 @@
       <c r="I696" t="s">
         <v>34</v>
       </c>
-      <c r="L696">
-        <v>20</v>
-      </c>
-      <c r="M696">
-        <v>7.31</v>
-      </c>
-      <c r="N696">
-        <v>17</v>
-      </c>
-      <c r="O696">
-        <v>8.51</v>
-      </c>
-    </row>
-    <row r="697" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J696" s="9">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="697" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A697" s="6">
         <v>1</v>
       </c>
@@ -19721,6 +19412,9 @@
       <c r="C697" s="7">
         <v>46068</v>
       </c>
+      <c r="D697" s="14">
+        <v>23.5</v>
+      </c>
       <c r="E697" s="9">
         <v>19.5</v>
       </c>
@@ -19733,20 +19427,11 @@
       <c r="H697" s="9">
         <v>12</v>
       </c>
-      <c r="L697">
-        <v>28</v>
-      </c>
-      <c r="M697">
-        <v>9.18</v>
-      </c>
-      <c r="N697">
-        <v>19</v>
-      </c>
-      <c r="O697">
-        <v>7.09</v>
-      </c>
-    </row>
-    <row r="698" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J697" s="9">
+        <v>8.1349999999999998</v>
+      </c>
+    </row>
+    <row r="698" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A698" s="6">
         <v>2</v>
       </c>
@@ -19756,6 +19441,9 @@
       <c r="C698" s="7">
         <v>46069</v>
       </c>
+      <c r="D698" s="14">
+        <v>12.5</v>
+      </c>
       <c r="E698" s="9">
         <v>23.5</v>
       </c>
@@ -19771,20 +19459,11 @@
       <c r="I698" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="L698">
-        <v>15</v>
-      </c>
-      <c r="M698">
-        <v>10.78</v>
-      </c>
-      <c r="N698">
-        <v>10</v>
-      </c>
-      <c r="O698">
-        <v>5.74</v>
-      </c>
-    </row>
-    <row r="699" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J698" s="9">
+        <v>8.26</v>
+      </c>
+    </row>
+    <row r="699" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A699" s="6">
         <v>3</v>
       </c>
@@ -19794,6 +19473,9 @@
       <c r="C699" s="7">
         <v>46070</v>
       </c>
+      <c r="D699" s="14">
+        <v>14.5</v>
+      </c>
       <c r="E699" s="9">
         <v>18.5</v>
       </c>
@@ -19806,20 +19488,11 @@
       <c r="H699" s="9">
         <v>4</v>
       </c>
-      <c r="L699">
-        <v>16</v>
-      </c>
-      <c r="M699">
-        <v>7.84</v>
-      </c>
-      <c r="N699">
-        <v>13</v>
-      </c>
-      <c r="O699">
-        <v>3.21</v>
-      </c>
-    </row>
-    <row r="700" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J699" s="9">
+        <v>5.5250000000000004</v>
+      </c>
+    </row>
+    <row r="700" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A700" s="6">
         <v>4</v>
       </c>
@@ -19829,6 +19502,9 @@
       <c r="C700" s="7">
         <v>46071</v>
       </c>
+      <c r="D700" s="14">
+        <v>15</v>
+      </c>
       <c r="E700" s="9">
         <v>20</v>
       </c>
@@ -19844,20 +19520,11 @@
       <c r="I700" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="L700">
-        <v>16</v>
-      </c>
-      <c r="M700">
-        <v>6.94</v>
-      </c>
-      <c r="N700">
-        <v>14</v>
-      </c>
-      <c r="O700">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="701" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J700" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="701" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A701" s="6">
         <v>5</v>
       </c>
@@ -19867,6 +19534,9 @@
       <c r="C701" s="7">
         <v>46072</v>
       </c>
+      <c r="D701" s="14">
+        <v>14.5</v>
+      </c>
       <c r="E701" s="9">
         <v>27.5</v>
       </c>
@@ -19879,20 +19549,11 @@
       <c r="H701" s="9">
         <v>6</v>
       </c>
-      <c r="L701">
-        <v>15</v>
-      </c>
-      <c r="M701">
-        <v>3.78</v>
-      </c>
-      <c r="N701">
-        <v>14</v>
-      </c>
-      <c r="O701">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="702" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J701" s="9">
+        <v>3.2149999999999999</v>
+      </c>
+    </row>
+    <row r="702" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A702" s="6">
         <v>6</v>
       </c>
@@ -19902,6 +19563,9 @@
       <c r="C702" s="7">
         <v>46073</v>
       </c>
+      <c r="D702" s="14">
+        <v>12</v>
+      </c>
       <c r="E702" s="9">
         <v>21.5</v>
       </c>
@@ -19917,20 +19581,11 @@
       <c r="I702" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L702">
-        <v>14</v>
-      </c>
-      <c r="M702">
-        <v>5.01</v>
-      </c>
-      <c r="N702">
-        <v>10</v>
-      </c>
-      <c r="O702">
-        <v>4.5599999999999996</v>
-      </c>
-    </row>
-    <row r="703" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J702" s="9">
+        <v>4.7850000000000001</v>
+      </c>
+    </row>
+    <row r="703" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A703" s="6">
         <v>7</v>
       </c>
@@ -19940,6 +19595,9 @@
       <c r="C703" s="7">
         <v>46074</v>
       </c>
+      <c r="D703" s="14">
+        <v>18.5</v>
+      </c>
       <c r="E703" s="9">
         <v>18.5</v>
       </c>
@@ -19952,20 +19610,11 @@
       <c r="H703" s="9">
         <v>13</v>
       </c>
-      <c r="L703">
-        <v>20</v>
-      </c>
-      <c r="M703">
-        <v>7.49</v>
-      </c>
-      <c r="N703">
-        <v>17</v>
-      </c>
-      <c r="O703">
-        <v>8.6</v>
-      </c>
-    </row>
-    <row r="704" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J703" s="9">
+        <v>8.0449999999999999</v>
+      </c>
+    </row>
+    <row r="704" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A704" s="6">
         <v>1</v>
       </c>
@@ -19975,6 +19624,9 @@
       <c r="C704" s="7">
         <v>46075</v>
       </c>
+      <c r="D704" s="14">
+        <v>23.5</v>
+      </c>
       <c r="E704" s="9">
         <v>20</v>
       </c>
@@ -19987,20 +19639,11 @@
       <c r="H704" s="9">
         <v>8</v>
       </c>
-      <c r="L704">
-        <v>30</v>
-      </c>
-      <c r="M704">
-        <v>13.98</v>
-      </c>
-      <c r="N704">
-        <v>17</v>
-      </c>
-      <c r="O704">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="705" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J704" s="9">
+        <v>9.4400000000000013</v>
+      </c>
+    </row>
+    <row r="705" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A705" s="6">
         <v>2</v>
       </c>
@@ -20010,6 +19653,9 @@
       <c r="C705" s="7">
         <v>46076</v>
       </c>
+      <c r="D705" s="14">
+        <v>10</v>
+      </c>
       <c r="E705" s="9">
         <v>22.5</v>
       </c>
@@ -20022,20 +19668,11 @@
       <c r="H705" s="9">
         <v>12</v>
       </c>
-      <c r="L705">
-        <v>13</v>
-      </c>
-      <c r="M705">
-        <v>7.24</v>
-      </c>
-      <c r="N705">
-        <v>7</v>
-      </c>
-      <c r="O705">
-        <v>2.62</v>
-      </c>
-    </row>
-    <row r="706" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J705" s="9">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="706" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A706" s="6">
         <v>3</v>
       </c>
@@ -20045,6 +19682,9 @@
       <c r="C706" s="7">
         <v>46077</v>
       </c>
+      <c r="D706" s="14">
+        <v>15.5</v>
+      </c>
       <c r="E706" s="9">
         <v>22.5</v>
       </c>
@@ -20057,20 +19697,11 @@
       <c r="H706" s="9">
         <v>5</v>
       </c>
-      <c r="L706">
-        <v>18</v>
-      </c>
-      <c r="M706">
-        <v>7.34</v>
-      </c>
-      <c r="N706">
-        <v>13</v>
-      </c>
-      <c r="O706">
-        <v>4.01</v>
-      </c>
-    </row>
-    <row r="707" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J706" s="9">
+        <v>5.6749999999999998</v>
+      </c>
+    </row>
+    <row r="707" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A707" s="6">
         <v>4</v>
       </c>
@@ -20080,6 +19711,9 @@
       <c r="C707" s="7">
         <v>46078</v>
       </c>
+      <c r="D707" s="14">
+        <v>8.5</v>
+      </c>
       <c r="E707" s="9">
         <v>26.5</v>
       </c>
@@ -20092,20 +19726,11 @@
       <c r="H707" s="9">
         <v>13</v>
       </c>
-      <c r="L707">
-        <v>10</v>
-      </c>
-      <c r="M707">
-        <v>4.6100000000000003</v>
-      </c>
-      <c r="N707">
-        <v>7</v>
-      </c>
-      <c r="O707">
-        <v>3.43</v>
-      </c>
-    </row>
-    <row r="708" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J707" s="9">
+        <v>4.0200000000000005</v>
+      </c>
+    </row>
+    <row r="708" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A708" s="6">
         <v>5</v>
       </c>
@@ -20115,6 +19740,9 @@
       <c r="C708" s="7">
         <v>46079</v>
       </c>
+      <c r="D708" s="14">
+        <v>15.5</v>
+      </c>
       <c r="E708" s="9">
         <v>20</v>
       </c>
@@ -20127,20 +19755,11 @@
       <c r="H708" s="9">
         <v>9</v>
       </c>
-      <c r="L708">
-        <v>17</v>
-      </c>
-      <c r="M708">
-        <v>5.23</v>
-      </c>
-      <c r="N708">
-        <v>14</v>
-      </c>
-      <c r="O708">
-        <v>5.93</v>
-      </c>
-    </row>
-    <row r="709" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J708" s="9">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="709" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A709" s="6">
         <v>6</v>
       </c>
@@ -20150,6 +19769,9 @@
       <c r="C709" s="7">
         <v>46080</v>
       </c>
+      <c r="D709" s="14">
+        <v>15.5</v>
+      </c>
       <c r="E709" s="9">
         <v>20.5</v>
       </c>
@@ -20165,20 +19787,11 @@
       <c r="I709" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L709">
-        <v>17</v>
-      </c>
-      <c r="M709">
-        <v>6.53</v>
-      </c>
-      <c r="N709">
-        <v>14</v>
-      </c>
-      <c r="O709">
-        <v>7.34</v>
-      </c>
-    </row>
-    <row r="710" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J709" s="9">
+        <v>6.9350000000000005</v>
+      </c>
+    </row>
+    <row r="710" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A710" s="6">
         <v>7</v>
       </c>
@@ -20188,6 +19801,9 @@
       <c r="C710" s="7">
         <v>46081</v>
       </c>
+      <c r="D710" s="14">
+        <v>18.5</v>
+      </c>
       <c r="E710" s="9">
         <v>25</v>
       </c>
@@ -20200,20 +19816,11 @@
       <c r="H710" s="9">
         <v>7</v>
       </c>
-      <c r="L710">
-        <v>19</v>
-      </c>
-      <c r="M710">
-        <v>5.6</v>
-      </c>
-      <c r="N710">
-        <v>18</v>
-      </c>
-      <c r="O710">
-        <v>6.34</v>
-      </c>
-    </row>
-    <row r="711" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J710" s="9">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="711" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A711" s="6">
         <v>1</v>
       </c>
@@ -20223,6 +19830,9 @@
       <c r="C711" s="7">
         <v>46082</v>
       </c>
+      <c r="D711" s="14">
+        <v>21</v>
+      </c>
       <c r="E711" s="9">
         <v>34</v>
       </c>
@@ -20235,20 +19845,11 @@
       <c r="H711" s="9">
         <v>14</v>
       </c>
-      <c r="L711">
-        <v>25</v>
-      </c>
-      <c r="M711">
-        <v>7.19</v>
-      </c>
-      <c r="N711">
-        <v>17</v>
-      </c>
-      <c r="O711">
-        <v>5.85</v>
-      </c>
-    </row>
-    <row r="712" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J711" s="9">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="712" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A712" s="6">
         <v>2</v>
       </c>
@@ -20258,6 +19859,9 @@
       <c r="C712" s="7">
         <v>46083</v>
       </c>
+      <c r="D712" s="14">
+        <v>20.5</v>
+      </c>
       <c r="E712" s="9">
         <v>30</v>
       </c>
@@ -20270,20 +19874,11 @@
       <c r="H712" s="9">
         <v>9</v>
       </c>
-      <c r="L712">
-        <v>24</v>
-      </c>
-      <c r="M712">
-        <v>6.64</v>
-      </c>
-      <c r="N712">
-        <v>17</v>
-      </c>
-      <c r="O712">
-        <v>5.77</v>
-      </c>
-    </row>
-    <row r="713" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J712" s="9">
+        <v>6.2050000000000001</v>
+      </c>
+    </row>
+    <row r="713" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A713" s="6">
         <v>3</v>
       </c>
@@ -20293,6 +19888,9 @@
       <c r="C713" s="7">
         <v>46084</v>
       </c>
+      <c r="D713" s="14">
+        <v>14.5</v>
+      </c>
       <c r="E713" s="9">
         <v>31</v>
       </c>
@@ -20305,20 +19903,11 @@
       <c r="H713" s="9">
         <v>8</v>
       </c>
-      <c r="L713">
-        <v>17</v>
-      </c>
-      <c r="M713">
-        <v>5.2</v>
-      </c>
-      <c r="N713">
-        <v>12</v>
-      </c>
-      <c r="O713">
-        <v>4.05</v>
-      </c>
-    </row>
-    <row r="714" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J713" s="9">
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="714" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A714" s="6">
         <v>4</v>
       </c>
@@ -20328,6 +19917,9 @@
       <c r="C714" s="7">
         <v>46085</v>
       </c>
+      <c r="D714" s="14">
+        <v>12</v>
+      </c>
       <c r="E714" s="9">
         <v>31</v>
       </c>
@@ -20340,20 +19932,11 @@
       <c r="H714" s="9">
         <v>22</v>
       </c>
-      <c r="L714">
-        <v>14</v>
-      </c>
-      <c r="M714">
-        <v>3.84</v>
-      </c>
-      <c r="N714">
-        <v>10</v>
-      </c>
-      <c r="O714">
-        <v>5.14</v>
-      </c>
-    </row>
-    <row r="715" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J714" s="9">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="715" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A715" s="6">
         <v>5</v>
       </c>
@@ -20363,6 +19946,9 @@
       <c r="C715" s="7">
         <v>46086</v>
       </c>
+      <c r="D715" s="14">
+        <v>21.5</v>
+      </c>
       <c r="E715" s="9">
         <v>32</v>
       </c>
@@ -20375,20 +19961,11 @@
       <c r="H715" s="9">
         <v>8</v>
       </c>
-      <c r="L715">
-        <v>23</v>
-      </c>
-      <c r="M715">
-        <v>7.03</v>
-      </c>
-      <c r="N715">
-        <v>20</v>
-      </c>
-      <c r="O715">
-        <v>8.2200000000000006</v>
-      </c>
-    </row>
-    <row r="716" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J715" s="9">
+        <v>7.625</v>
+      </c>
+    </row>
+    <row r="716" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A716" s="6">
         <v>6</v>
       </c>
@@ -20398,6 +19975,9 @@
       <c r="C716" s="7">
         <v>46087</v>
       </c>
+      <c r="D716" s="14">
+        <v>9.5</v>
+      </c>
       <c r="E716" s="9">
         <v>37.5</v>
       </c>
@@ -20413,20 +19993,11 @@
       <c r="I716" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L716">
-        <v>10</v>
-      </c>
-      <c r="M716">
-        <v>2.69</v>
-      </c>
-      <c r="N716">
-        <v>9</v>
-      </c>
-      <c r="O716">
-        <v>3.56</v>
-      </c>
-    </row>
-    <row r="717" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J716" s="9">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="717" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A717" s="6">
         <v>7</v>
       </c>
@@ -20436,6 +20007,9 @@
       <c r="C717" s="7">
         <v>46088</v>
       </c>
+      <c r="D717" s="14">
+        <v>26.5</v>
+      </c>
       <c r="E717" s="9">
         <v>39</v>
       </c>
@@ -20448,26 +20022,17 @@
       <c r="H717" s="9">
         <v>16</v>
       </c>
-      <c r="L717">
-        <v>28</v>
-      </c>
-      <c r="M717">
-        <v>9.58</v>
-      </c>
-      <c r="N717">
-        <v>25</v>
-      </c>
-      <c r="O717">
-        <v>12.05</v>
-      </c>
-    </row>
-    <row r="718" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J717" s="9">
+        <v>10.815000000000001</v>
+      </c>
+    </row>
+    <row r="718" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A718" s="6"/>
     </row>
-    <row r="719" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A719" s="6"/>
     </row>
-    <row r="720" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A720" s="6"/>
     </row>
     <row r="721" spans="1:1" x14ac:dyDescent="0.25">
@@ -20486,8 +20051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6638D5E3-C858-457D-8856-EE1DEA6B94D7}">
   <dimension ref="A1:S257"/>
   <sheetViews>
-    <sheetView topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="O196" sqref="O196:P251"/>
+    <sheetView topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="Q196" sqref="Q196:Q219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20500,20 +20065,20 @@
         <v>43</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="39">
+      <c r="C1" s="41">
         <v>0.85</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="43"/>
       <c r="O1" s="22" t="s">
         <v>39</v>
       </c>
@@ -28285,7 +27850,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q195" t="e">
-        <f t="shared" ref="Q195:Q196" si="13">O195-A195</f>
+        <f t="shared" ref="Q195:Q219" si="13">O195-A195</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -28352,6 +27917,9 @@
       </c>
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>7</v>
+      </c>
       <c r="B197" s="24">
         <v>46034</v>
       </c>
@@ -28399,6 +27967,10 @@
         <f t="shared" si="12"/>
         <v>6.82</v>
       </c>
+      <c r="Q197">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
       <c r="R197">
         <v>41</v>
       </c>
@@ -28407,6 +27979,9 @@
       </c>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>2</v>
+      </c>
       <c r="B198" s="24">
         <v>46035</v>
       </c>
@@ -28454,6 +28029,10 @@
         <f t="shared" si="12"/>
         <v>6.73</v>
       </c>
+      <c r="Q198">
+        <f t="shared" si="13"/>
+        <v>24</v>
+      </c>
       <c r="R198">
         <v>39</v>
       </c>
@@ -28462,6 +28041,9 @@
       </c>
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>21</v>
+      </c>
       <c r="B199" s="24">
         <v>46036</v>
       </c>
@@ -28509,6 +28091,10 @@
         <f t="shared" si="12"/>
         <v>6.17</v>
       </c>
+      <c r="Q199">
+        <f t="shared" si="13"/>
+        <v>-5</v>
+      </c>
       <c r="R199">
         <v>28</v>
       </c>
@@ -28517,6 +28103,9 @@
       </c>
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>11</v>
+      </c>
       <c r="B200" s="24">
         <v>46037</v>
       </c>
@@ -28564,6 +28153,10 @@
         <f t="shared" si="12"/>
         <v>4.99</v>
       </c>
+      <c r="Q200">
+        <f t="shared" si="13"/>
+        <v>-2</v>
+      </c>
       <c r="R200">
         <v>26</v>
       </c>
@@ -28572,6 +28165,9 @@
       </c>
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>0</v>
+      </c>
       <c r="B201" s="24">
         <v>46038</v>
       </c>
@@ -28619,6 +28215,10 @@
         <f t="shared" si="12"/>
         <v>12.42</v>
       </c>
+      <c r="Q201">
+        <f t="shared" si="13"/>
+        <v>29</v>
+      </c>
       <c r="R201">
         <v>42</v>
       </c>
@@ -28627,6 +28227,9 @@
       </c>
     </row>
     <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>15</v>
+      </c>
       <c r="B202" s="24">
         <v>46039</v>
       </c>
@@ -28674,6 +28277,10 @@
         <f t="shared" si="12"/>
         <v>4.6900000000000004</v>
       </c>
+      <c r="Q202">
+        <f t="shared" si="13"/>
+        <v>-2</v>
+      </c>
       <c r="R202">
         <v>21</v>
       </c>
@@ -28682,6 +28289,9 @@
       </c>
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>25</v>
+      </c>
       <c r="B203" s="24">
         <v>46040</v>
       </c>
@@ -28729,6 +28339,10 @@
         <f t="shared" si="12"/>
         <v>10.25</v>
       </c>
+      <c r="Q203">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
       <c r="R203">
         <v>62</v>
       </c>
@@ -28737,6 +28351,9 @@
       </c>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>21</v>
+      </c>
       <c r="B204" s="24">
         <v>46041</v>
       </c>
@@ -28784,6 +28401,10 @@
         <f t="shared" ref="P204:P251" si="15">ROUND(_xlfn.STDEV.P(C204:N204,R204,S204),2)</f>
         <v>9.69</v>
       </c>
+      <c r="Q204">
+        <f t="shared" si="13"/>
+        <v>-10</v>
+      </c>
       <c r="R204">
         <v>39</v>
       </c>
@@ -28792,6 +28413,9 @@
       </c>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>5</v>
+      </c>
       <c r="B205" s="24">
         <v>46042</v>
       </c>
@@ -28839,6 +28463,10 @@
         <f t="shared" si="15"/>
         <v>9.01</v>
       </c>
+      <c r="Q205">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
       <c r="R205">
         <v>38</v>
       </c>
@@ -28847,6 +28475,9 @@
       </c>
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>18</v>
+      </c>
       <c r="B206" s="24">
         <v>46043</v>
       </c>
@@ -28894,6 +28525,10 @@
         <f t="shared" si="15"/>
         <v>5.9</v>
       </c>
+      <c r="Q206">
+        <f t="shared" si="13"/>
+        <v>-1</v>
+      </c>
       <c r="R206">
         <v>33</v>
       </c>
@@ -28902,6 +28537,9 @@
       </c>
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>12</v>
+      </c>
       <c r="B207" s="24">
         <v>46044</v>
       </c>
@@ -28949,6 +28587,10 @@
         <f t="shared" si="15"/>
         <v>5.37</v>
       </c>
+      <c r="Q207">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
       <c r="R207">
         <v>32</v>
       </c>
@@ -28957,6 +28599,9 @@
       </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>7</v>
+      </c>
       <c r="B208" s="24">
         <v>46045</v>
       </c>
@@ -29004,6 +28649,10 @@
         <f t="shared" si="15"/>
         <v>5.14</v>
       </c>
+      <c r="Q208">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
       <c r="R208">
         <v>22</v>
       </c>
@@ -29011,7 +28660,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>26</v>
+      </c>
       <c r="B209" s="24">
         <v>46046</v>
       </c>
@@ -29059,6 +28711,10 @@
         <f t="shared" si="15"/>
         <v>7.81</v>
       </c>
+      <c r="Q209">
+        <f t="shared" si="13"/>
+        <v>-7</v>
+      </c>
       <c r="R209">
         <v>25</v>
       </c>
@@ -29066,7 +28722,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>36</v>
+      </c>
       <c r="B210" s="24">
         <v>46047</v>
       </c>
@@ -29114,6 +28773,10 @@
         <f t="shared" si="15"/>
         <v>14.02</v>
       </c>
+      <c r="Q210">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
       <c r="R210">
         <v>74</v>
       </c>
@@ -29121,7 +28784,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="211" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>11</v>
+      </c>
       <c r="B211" s="24">
         <v>46048</v>
       </c>
@@ -29169,6 +28835,10 @@
         <f t="shared" si="15"/>
         <v>12.02</v>
       </c>
+      <c r="Q211">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
       <c r="R211">
         <v>59</v>
       </c>
@@ -29176,7 +28846,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="212" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>9</v>
+      </c>
       <c r="B212" s="24">
         <v>46049</v>
       </c>
@@ -29224,6 +28897,10 @@
         <f t="shared" si="15"/>
         <v>10.19</v>
       </c>
+      <c r="Q212">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
       <c r="R212">
         <v>39</v>
       </c>
@@ -29231,7 +28908,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>14</v>
+      </c>
       <c r="B213" s="24">
         <v>46050</v>
       </c>
@@ -29279,6 +28959,10 @@
         <f t="shared" si="15"/>
         <v>5.7</v>
       </c>
+      <c r="Q213">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
       <c r="R213">
         <v>31</v>
       </c>
@@ -29286,7 +28970,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="214" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>10</v>
+      </c>
       <c r="B214" s="24">
         <v>46051</v>
       </c>
@@ -29334,6 +29021,10 @@
         <f t="shared" si="15"/>
         <v>5.25</v>
       </c>
+      <c r="Q214">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
       <c r="R214">
         <v>26</v>
       </c>
@@ -29341,7 +29032,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="215" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>19</v>
+      </c>
       <c r="B215" s="24">
         <v>46052</v>
       </c>
@@ -29389,6 +29083,10 @@
         <f t="shared" si="15"/>
         <v>9.6300000000000008</v>
       </c>
+      <c r="Q215">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
       <c r="R215">
         <v>25</v>
       </c>
@@ -29396,7 +29094,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="216" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>28</v>
+      </c>
       <c r="B216" s="24">
         <v>46053</v>
       </c>
@@ -29444,6 +29145,10 @@
         <f t="shared" si="15"/>
         <v>5.73</v>
       </c>
+      <c r="Q216">
+        <f t="shared" si="13"/>
+        <v>-10</v>
+      </c>
       <c r="R216">
         <v>27</v>
       </c>
@@ -29451,7 +29156,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="217" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>11</v>
+      </c>
       <c r="B217" s="24">
         <v>46054</v>
       </c>
@@ -29499,6 +29207,10 @@
         <f t="shared" si="15"/>
         <v>9.32</v>
       </c>
+      <c r="Q217">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
       <c r="R217">
         <v>54</v>
       </c>
@@ -29506,7 +29218,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="218" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>4</v>
+      </c>
       <c r="B218" s="24">
         <v>46055</v>
       </c>
@@ -29554,6 +29269,10 @@
         <f t="shared" si="15"/>
         <v>6.52</v>
       </c>
+      <c r="Q218">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
       <c r="R218">
         <v>31</v>
       </c>
@@ -29561,7 +29280,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>1</v>
+      </c>
       <c r="B219" s="24">
         <v>46056</v>
       </c>
@@ -29609,6 +29331,10 @@
         <f t="shared" si="15"/>
         <v>9.17</v>
       </c>
+      <c r="Q219">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
       <c r="R219">
         <v>40</v>
       </c>
@@ -29616,7 +29342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B220" s="24">
         <v>46057</v>
       </c>
@@ -29671,7 +29397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="221" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B221" s="24">
         <v>46058</v>
       </c>
@@ -29726,7 +29452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="222" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B222" s="24">
         <v>46059</v>
       </c>
@@ -29781,7 +29507,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="223" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B223" s="24">
         <v>46060</v>
       </c>
@@ -29836,7 +29562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B224" s="24">
         <v>46061</v>
       </c>
@@ -31488,34 +31214,34 @@
     </row>
     <row r="254" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B254" s="24"/>
-      <c r="C254" s="38" t="s">
+      <c r="C254" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D254" s="38"/>
-      <c r="E254" s="38" t="s">
+      <c r="D254" s="40"/>
+      <c r="E254" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="F254" s="38"/>
-      <c r="G254" s="38" t="s">
+      <c r="F254" s="40"/>
+      <c r="G254" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H254" s="38"/>
-      <c r="I254" s="38" t="s">
+      <c r="H254" s="40"/>
+      <c r="I254" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="J254" s="38"/>
-      <c r="K254" s="42" t="s">
+      <c r="J254" s="40"/>
+      <c r="K254" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="L254" s="42"/>
-      <c r="M254" s="42" t="s">
+      <c r="L254" s="44"/>
+      <c r="M254" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="N254" s="42"/>
-      <c r="R254" s="38" t="s">
+      <c r="N254" s="44"/>
+      <c r="R254" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="S254" s="38"/>
+      <c r="S254" s="40"/>
     </row>
     <row r="255" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C255" t="s">
@@ -31612,34 +31338,34 @@
       <c r="B257" t="s">
         <v>58</v>
       </c>
-      <c r="C257" s="44"/>
-      <c r="D257" s="44"/>
-      <c r="E257" s="44"/>
-      <c r="F257" s="44"/>
-      <c r="G257" s="44"/>
-      <c r="H257" s="44"/>
-      <c r="I257" s="45">
+      <c r="C257" s="38"/>
+      <c r="D257" s="38"/>
+      <c r="E257" s="38"/>
+      <c r="F257" s="38"/>
+      <c r="G257" s="38"/>
+      <c r="H257" s="38"/>
+      <c r="I257" s="39">
         <v>0.80600000000000005</v>
       </c>
-      <c r="J257" s="45">
+      <c r="J257" s="39">
         <v>0.77400000000000002</v>
       </c>
-      <c r="K257" s="45">
+      <c r="K257" s="39">
         <v>0.80300000000000005</v>
       </c>
-      <c r="L257" s="45">
+      <c r="L257" s="39">
         <v>0.70799999999999996</v>
       </c>
-      <c r="M257" s="45">
+      <c r="M257" s="39">
         <v>0.80300000000000005</v>
       </c>
-      <c r="N257" s="45">
+      <c r="N257" s="39">
         <v>0.85699999999999998</v>
       </c>
-      <c r="R257" s="45">
+      <c r="R257" s="39">
         <v>0.73499999999999999</v>
       </c>
-      <c r="S257" s="45">
+      <c r="S257" s="39">
         <v>0.74099999999999999</v>
       </c>
     </row>
@@ -31665,7 +31391,7 @@
       <formula>ABS(C116-$A116)&lt;=10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q196">
+  <conditionalFormatting sqref="Q1:Q219">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -31681,8 +31407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2573A6AB-8DBE-4210-8EFE-4E449AA3F45B}">
   <dimension ref="A1:S252"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O196" sqref="O196:P251"/>
+    <sheetView topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q219" sqref="Q196:Q219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31695,20 +31421,20 @@
         <v>43</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="39">
+      <c r="C1" s="41">
         <v>0.85</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="43"/>
       <c r="O1" s="22" t="s">
         <v>39</v>
       </c>
@@ -39373,7 +39099,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q195" t="e">
-        <f t="shared" ref="Q195:Q196" si="12">O195-A195</f>
+        <f t="shared" ref="Q195:Q219" si="12">O195-A195</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -39440,6 +39166,9 @@
       </c>
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>7</v>
+      </c>
       <c r="B197" s="24">
         <v>46034</v>
       </c>
@@ -39487,6 +39216,10 @@
         <f t="shared" si="11"/>
         <v>6.05</v>
       </c>
+      <c r="Q197">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
       <c r="R197">
         <v>9</v>
       </c>
@@ -39495,6 +39228,9 @@
       </c>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>2</v>
+      </c>
       <c r="B198" s="24">
         <v>46035</v>
       </c>
@@ -39542,6 +39278,10 @@
         <f t="shared" si="11"/>
         <v>9.24</v>
       </c>
+      <c r="Q198">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
       <c r="R198">
         <v>17</v>
       </c>
@@ -39550,6 +39290,9 @@
       </c>
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>21</v>
+      </c>
       <c r="B199" s="24">
         <v>46036</v>
       </c>
@@ -39597,6 +39340,10 @@
         <f t="shared" si="11"/>
         <v>4.8099999999999996</v>
       </c>
+      <c r="Q199">
+        <f t="shared" si="12"/>
+        <v>-9</v>
+      </c>
       <c r="R199">
         <v>10</v>
       </c>
@@ -39605,6 +39352,9 @@
       </c>
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>11</v>
+      </c>
       <c r="B200" s="24">
         <v>46037</v>
       </c>
@@ -39652,6 +39402,10 @@
         <f t="shared" si="11"/>
         <v>2.41</v>
       </c>
+      <c r="Q200">
+        <f t="shared" si="12"/>
+        <v>-4</v>
+      </c>
       <c r="R200">
         <v>4</v>
       </c>
@@ -39660,6 +39414,9 @@
       </c>
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>0</v>
+      </c>
       <c r="B201" s="24">
         <v>46038</v>
       </c>
@@ -39707,6 +39464,10 @@
         <f t="shared" si="11"/>
         <v>13.75</v>
       </c>
+      <c r="Q201">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
       <c r="R201">
         <v>18</v>
       </c>
@@ -39715,6 +39476,9 @@
       </c>
     </row>
     <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>15</v>
+      </c>
       <c r="B202" s="24">
         <v>46039</v>
       </c>
@@ -39762,6 +39526,10 @@
         <f t="shared" si="11"/>
         <v>4.88</v>
       </c>
+      <c r="Q202">
+        <f t="shared" si="12"/>
+        <v>-5</v>
+      </c>
       <c r="R202">
         <v>8</v>
       </c>
@@ -39770,6 +39538,9 @@
       </c>
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>25</v>
+      </c>
       <c r="B203" s="24">
         <v>46040</v>
       </c>
@@ -39817,6 +39588,10 @@
         <f t="shared" si="11"/>
         <v>6.58</v>
       </c>
+      <c r="Q203">
+        <f t="shared" si="12"/>
+        <v>-5</v>
+      </c>
       <c r="R203">
         <v>18</v>
       </c>
@@ -39825,6 +39600,9 @@
       </c>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>21</v>
+      </c>
       <c r="B204" s="24">
         <v>46041</v>
       </c>
@@ -39872,6 +39650,10 @@
         <f t="shared" ref="P204:P251" si="14">ROUND(_xlfn.STDEV.P(C204:N204,R204,S204),2)</f>
         <v>3.22</v>
       </c>
+      <c r="Q204">
+        <f t="shared" si="12"/>
+        <v>-15</v>
+      </c>
       <c r="R204">
         <v>6</v>
       </c>
@@ -39880,6 +39662,9 @@
       </c>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>5</v>
+      </c>
       <c r="B205" s="24">
         <v>46042</v>
       </c>
@@ -39927,6 +39712,10 @@
         <f t="shared" si="14"/>
         <v>4.6399999999999997</v>
       </c>
+      <c r="Q205">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
       <c r="R205">
         <v>6</v>
       </c>
@@ -39935,6 +39724,9 @@
       </c>
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>18</v>
+      </c>
       <c r="B206" s="24">
         <v>46043</v>
       </c>
@@ -39982,6 +39774,10 @@
         <f t="shared" si="14"/>
         <v>5.37</v>
       </c>
+      <c r="Q206">
+        <f t="shared" si="12"/>
+        <v>-5</v>
+      </c>
       <c r="R206">
         <v>13</v>
       </c>
@@ -39990,6 +39786,9 @@
       </c>
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>12</v>
+      </c>
       <c r="B207" s="24">
         <v>46044</v>
       </c>
@@ -40037,6 +39836,10 @@
         <f t="shared" si="14"/>
         <v>5.36</v>
       </c>
+      <c r="Q207">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
       <c r="R207">
         <v>12</v>
       </c>
@@ -40045,6 +39848,9 @@
       </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>7</v>
+      </c>
       <c r="B208" s="24">
         <v>46045</v>
       </c>
@@ -40092,6 +39898,10 @@
         <f t="shared" si="14"/>
         <v>5.36</v>
       </c>
+      <c r="Q208">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
       <c r="R208">
         <v>10</v>
       </c>
@@ -40099,7 +39909,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="209" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>26</v>
+      </c>
       <c r="B209" s="24">
         <v>46046</v>
       </c>
@@ -40147,6 +39960,10 @@
         <f t="shared" si="14"/>
         <v>8.8699999999999992</v>
       </c>
+      <c r="Q209">
+        <f t="shared" si="12"/>
+        <v>-10</v>
+      </c>
       <c r="R209">
         <v>14</v>
       </c>
@@ -40154,7 +39971,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>36</v>
+      </c>
       <c r="B210" s="24">
         <v>46047</v>
       </c>
@@ -40202,6 +40022,10 @@
         <f t="shared" si="14"/>
         <v>6.8</v>
       </c>
+      <c r="Q210">
+        <f t="shared" si="12"/>
+        <v>-7</v>
+      </c>
       <c r="R210">
         <v>27</v>
       </c>
@@ -40209,7 +40033,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="211" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>11</v>
+      </c>
       <c r="B211" s="24">
         <v>46048</v>
       </c>
@@ -40257,6 +40084,10 @@
         <f t="shared" si="14"/>
         <v>6.87</v>
       </c>
+      <c r="Q211">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
       <c r="R211">
         <v>14</v>
       </c>
@@ -40264,7 +40095,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>9</v>
+      </c>
       <c r="B212" s="24">
         <v>46049</v>
       </c>
@@ -40312,6 +40146,10 @@
         <f t="shared" si="14"/>
         <v>3.77</v>
       </c>
+      <c r="Q212">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
       <c r="R212">
         <v>8</v>
       </c>
@@ -40319,7 +40157,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>14</v>
+      </c>
       <c r="B213" s="24">
         <v>46050</v>
       </c>
@@ -40367,6 +40208,10 @@
         <f t="shared" si="14"/>
         <v>4.3899999999999997</v>
       </c>
+      <c r="Q213">
+        <f t="shared" si="12"/>
+        <v>-3</v>
+      </c>
       <c r="R213">
         <v>11</v>
       </c>
@@ -40374,7 +40219,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>10</v>
+      </c>
       <c r="B214" s="24">
         <v>46051</v>
       </c>
@@ -40422,6 +40270,10 @@
         <f t="shared" si="14"/>
         <v>4.3499999999999996</v>
       </c>
+      <c r="Q214">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
       <c r="R214">
         <v>12</v>
       </c>
@@ -40429,7 +40281,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="215" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>19</v>
+      </c>
       <c r="B215" s="24">
         <v>46052</v>
       </c>
@@ -40477,6 +40332,10 @@
         <f t="shared" si="14"/>
         <v>11.08</v>
       </c>
+      <c r="Q215">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
       <c r="R215">
         <v>14</v>
       </c>
@@ -40484,7 +40343,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="216" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>28</v>
+      </c>
       <c r="B216" s="24">
         <v>46053</v>
       </c>
@@ -40532,6 +40394,10 @@
         <f t="shared" si="14"/>
         <v>7.18</v>
       </c>
+      <c r="Q216">
+        <f t="shared" si="12"/>
+        <v>-13</v>
+      </c>
       <c r="R216">
         <v>12</v>
       </c>
@@ -40539,7 +40405,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>11</v>
+      </c>
       <c r="B217" s="24">
         <v>46054</v>
       </c>
@@ -40587,6 +40456,10 @@
         <f t="shared" si="14"/>
         <v>7.73</v>
       </c>
+      <c r="Q217">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
       <c r="R217">
         <v>16</v>
       </c>
@@ -40594,7 +40467,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>4</v>
+      </c>
       <c r="B218" s="24">
         <v>46055</v>
       </c>
@@ -40642,6 +40518,10 @@
         <f t="shared" si="14"/>
         <v>2.17</v>
       </c>
+      <c r="Q218">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
       <c r="R218">
         <v>4</v>
       </c>
@@ -40649,7 +40529,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>1</v>
+      </c>
       <c r="B219" s="24">
         <v>46056</v>
       </c>
@@ -40697,6 +40580,10 @@
         <f t="shared" si="14"/>
         <v>2.94</v>
       </c>
+      <c r="Q219">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
       <c r="R219">
         <v>11</v>
       </c>
@@ -40704,7 +40591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="220" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B220" s="24">
         <v>46057</v>
       </c>
@@ -40759,7 +40646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B221" s="24">
         <v>46058</v>
       </c>
@@ -40814,7 +40701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B222" s="24">
         <v>46059</v>
       </c>
@@ -40869,7 +40756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B223" s="24">
         <v>46060</v>
       </c>
@@ -40924,7 +40811,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="224" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B224" s="24">
         <v>46061</v>
       </c>
@@ -42466,37 +42353,37 @@
     </row>
     <row r="252" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B252" s="32"/>
-      <c r="C252" s="43" t="s">
+      <c r="C252" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D252" s="43"/>
-      <c r="E252" s="43" t="s">
+      <c r="D252" s="45"/>
+      <c r="E252" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F252" s="43"/>
-      <c r="G252" s="43" t="s">
+      <c r="F252" s="45"/>
+      <c r="G252" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="H252" s="43"/>
-      <c r="I252" s="43" t="s">
+      <c r="H252" s="45"/>
+      <c r="I252" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="J252" s="43"/>
-      <c r="K252" s="43" t="s">
+      <c r="J252" s="45"/>
+      <c r="K252" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="L252" s="43"/>
-      <c r="M252" s="43" t="s">
+      <c r="L252" s="45"/>
+      <c r="M252" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="N252" s="43"/>
+      <c r="N252" s="45"/>
       <c r="O252" s="32"/>
       <c r="P252" s="32"/>
       <c r="Q252" s="32"/>
-      <c r="R252" s="43" t="s">
+      <c r="R252" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="S252" s="43"/>
+      <c r="S252" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -42509,15 +42396,15 @@
     <mergeCell ref="I252:J252"/>
     <mergeCell ref="K252:L252"/>
   </mergeCells>
+  <conditionalFormatting sqref="C81">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C116:O121">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>ABS(C116-$A116)&lt;=10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q196">
+  <conditionalFormatting sqref="Q1:Q219">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>